<commit_message>
added mapf, steinlib random terminals, but not passing steinlib 15
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -493,22 +493,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2319.57</v>
+        <v>59.452</v>
       </c>
       <c r="C2">
-        <v>100.732</v>
+        <v>50.59199999999999</v>
       </c>
       <c r="D2">
-        <v>100.732</v>
+        <v>50.59199999999999</v>
       </c>
       <c r="E2">
-        <v>100.732</v>
+        <v>50.59199999999999</v>
       </c>
       <c r="F2">
-        <v>100.732</v>
+        <v>50.59199999999999</v>
       </c>
       <c r="G2">
-        <v>0.7652583884081964</v>
+        <v>0.1192222296979077</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -528,22 +528,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2447.078</v>
+        <v>20.726</v>
       </c>
       <c r="C3">
-        <v>105.42</v>
+        <v>42.038</v>
       </c>
       <c r="D3">
-        <v>105.42</v>
+        <v>42.038</v>
       </c>
       <c r="E3">
-        <v>105.42</v>
+        <v>42.038</v>
       </c>
       <c r="F3">
-        <v>105.42</v>
+        <v>42.038</v>
       </c>
       <c r="G3">
-        <v>0.7655360393089227</v>
+        <v>0.8226189327414839</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -563,22 +563,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2725.865999999999</v>
+        <v>61.796</v>
       </c>
       <c r="C4">
-        <v>117.872</v>
+        <v>54.55399999999999</v>
       </c>
       <c r="D4">
-        <v>117.872</v>
+        <v>54.554</v>
       </c>
       <c r="E4">
-        <v>117.872</v>
+        <v>54.554</v>
       </c>
       <c r="F4">
-        <v>117.872</v>
+        <v>54.554</v>
       </c>
       <c r="G4">
-        <v>0.7654063699389478</v>
+        <v>0.09375364101236328</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -598,22 +598,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2648.318</v>
+        <v>40.108</v>
       </c>
       <c r="C5">
-        <v>113.076</v>
+        <v>37.14</v>
       </c>
       <c r="D5">
-        <v>113.076</v>
+        <v>37.14</v>
       </c>
       <c r="E5">
-        <v>113.076</v>
+        <v>37.14</v>
       </c>
       <c r="F5">
-        <v>113.076</v>
+        <v>37.14</v>
       </c>
       <c r="G5">
-        <v>0.7658421685009127</v>
+        <v>0.05920015956916314</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -633,22 +633,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2376.384</v>
+        <v>41.554</v>
       </c>
       <c r="C6">
-        <v>103.076</v>
+        <v>65.79599999999999</v>
       </c>
       <c r="D6">
-        <v>103.076</v>
+        <v>65.79599999999999</v>
       </c>
       <c r="E6">
-        <v>103.076</v>
+        <v>65.79599999999999</v>
       </c>
       <c r="F6">
-        <v>103.076</v>
+        <v>65.79599999999999</v>
       </c>
       <c r="G6">
-        <v>0.7652998841938004</v>
+        <v>0.4667083794580542</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -713,31 +713,31 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>88</v>
+        <v>1840</v>
       </c>
       <c r="D2">
-        <v>0.009406106546521187</v>
+        <v>0.02247039030771703</v>
       </c>
       <c r="E2">
-        <v>0.09662567399209365</v>
+        <v>0.7443019769852981</v>
       </c>
       <c r="F2">
-        <v>88</v>
+        <v>1840</v>
       </c>
       <c r="G2">
-        <v>0.00352320569800213</v>
+        <v>0.05537386040668935</v>
       </c>
       <c r="H2">
-        <v>0.03519146679900587</v>
+        <v>0.4904221027391031</v>
       </c>
       <c r="I2">
-        <v>0.02229262614855543</v>
+        <v>0.03413118747994304</v>
       </c>
       <c r="J2">
-        <v>0.03155661298660561</v>
+        <v>0.08356877986807376</v>
       </c>
       <c r="K2">
-        <v>0.001083862851373851</v>
+        <v>0.01999597204849124</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -746,31 +746,31 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>956</v>
+        <v>866</v>
       </c>
       <c r="D3">
-        <v>0.001377664098981768</v>
+        <v>0.0009043698664754629</v>
       </c>
       <c r="E3">
-        <v>0.457222823984921</v>
+        <v>0.3264306769706309</v>
       </c>
       <c r="F3">
-        <v>956</v>
+        <v>866</v>
       </c>
       <c r="G3">
-        <v>0.03401386545738205</v>
+        <v>0.02500208560377359</v>
       </c>
       <c r="H3">
-        <v>0.2476836052373983</v>
+        <v>0.2106004991801456</v>
       </c>
       <c r="I3">
-        <v>0.03663229115772992</v>
+        <v>0.007719359477050602</v>
       </c>
       <c r="J3">
-        <v>0.0942635660758242</v>
+        <v>0.04627484793309122</v>
       </c>
       <c r="K3">
-        <v>0.01129332842538133</v>
+        <v>0.009199967258609831</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -779,31 +779,31 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>866</v>
       </c>
       <c r="D4">
-        <v>0.009509444353170693</v>
+        <v>0.009958986309356987</v>
       </c>
       <c r="E4">
-        <v>0.09698447503615171</v>
+        <v>0.3579659190727398</v>
       </c>
       <c r="F4">
-        <v>89</v>
+        <v>866</v>
       </c>
       <c r="G4">
-        <v>0.003538834338542074</v>
+        <v>0.02703198709059507</v>
       </c>
       <c r="H4">
-        <v>0.03566912829410285</v>
+        <v>0.2321864258265123</v>
       </c>
       <c r="I4">
-        <v>0.02235741110052913</v>
+        <v>0.009908543550409377</v>
       </c>
       <c r="J4">
-        <v>0.03131848305929452</v>
+        <v>0.04946563148405403</v>
       </c>
       <c r="K4">
-        <v>0.001062801107764244</v>
+        <v>0.009843050269410014</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -812,31 +812,31 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>956</v>
+        <v>866</v>
       </c>
       <c r="D5">
-        <v>0.002050002396572381</v>
+        <v>0.001394452061504126</v>
       </c>
       <c r="E5">
-        <v>0.4581472249701619</v>
+        <v>0.3342486170586199</v>
       </c>
       <c r="F5">
-        <v>956</v>
+        <v>866</v>
       </c>
       <c r="G5">
-        <v>0.03343825676711276</v>
+        <v>0.02607315022032708</v>
       </c>
       <c r="H5">
-        <v>0.2467607537982985</v>
+        <v>0.2134779418120161</v>
       </c>
       <c r="I5">
-        <v>0.03968676587101072</v>
+        <v>0.008885901304893196</v>
       </c>
       <c r="J5">
-        <v>0.09413713944377378</v>
+        <v>0.04743586608674377</v>
       </c>
       <c r="K5">
-        <v>0.01098228478804231</v>
+        <v>0.009680040297098458</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -845,10 +845,10 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>24025</v>
+        <v>4805</v>
       </c>
       <c r="E6">
-        <v>4.53717471397249</v>
+        <v>0.9688141721999273</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -859,31 +859,31 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>89</v>
+        <v>1563</v>
       </c>
       <c r="D7">
-        <v>0.009881724137812853</v>
+        <v>0.01898405444808304</v>
       </c>
       <c r="E7">
-        <v>0.1001604669727385</v>
+        <v>0.6381196749862283</v>
       </c>
       <c r="F7">
-        <v>89</v>
+        <v>1563</v>
       </c>
       <c r="G7">
-        <v>0.003448279108852148</v>
+        <v>0.04755687050055712</v>
       </c>
       <c r="H7">
-        <v>0.03651109209749848</v>
+        <v>0.4147311503766105</v>
       </c>
       <c r="I7">
-        <v>0.0230383159359917</v>
+        <v>0.03226113377604634</v>
       </c>
       <c r="J7">
-        <v>0.03303361096186563</v>
+        <v>0.07299588446039706</v>
       </c>
       <c r="K7">
-        <v>0.001076423155609518</v>
+        <v>0.01736028608866036</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -892,31 +892,31 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>1076</v>
+        <v>707</v>
       </c>
       <c r="D8">
-        <v>0.001588479848578572</v>
+        <v>0.000774587388150394</v>
       </c>
       <c r="E8">
-        <v>0.5320628189947456</v>
+        <v>0.2742936819558963</v>
       </c>
       <c r="F8">
-        <v>1076</v>
+        <v>707</v>
       </c>
       <c r="G8">
-        <v>0.03883406618842855</v>
+        <v>0.0207951336633414</v>
       </c>
       <c r="H8">
-        <v>0.2868864864576608</v>
+        <v>0.1727409242885187</v>
       </c>
       <c r="I8">
-        <v>0.0427607077290304</v>
+        <v>0.008141346508637071</v>
       </c>
       <c r="J8">
-        <v>0.1123834900790825</v>
+        <v>0.04147404141258448</v>
       </c>
       <c r="K8">
-        <v>0.01268269715365022</v>
+        <v>0.007689272402785718</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -925,31 +925,31 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>89</v>
+        <v>707</v>
       </c>
       <c r="D9">
-        <v>0.009883266349788755</v>
+        <v>0.009927223902195692</v>
       </c>
       <c r="E9">
-        <v>0.0991096890065819</v>
+        <v>0.3200639389688149</v>
       </c>
       <c r="F9">
-        <v>89</v>
+        <v>707</v>
       </c>
       <c r="G9">
-        <v>0.003378540102858096</v>
+        <v>0.02328084665350616</v>
       </c>
       <c r="H9">
-        <v>0.03573820018209517</v>
+        <v>0.2040852522477508</v>
       </c>
       <c r="I9">
-        <v>0.02302630915073678</v>
+        <v>0.01169244933407754</v>
       </c>
       <c r="J9">
-        <v>0.03292750183027238</v>
+        <v>0.04653520707506686</v>
       </c>
       <c r="K9">
-        <v>0.001059138798154891</v>
+        <v>0.008607124909758568</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -958,31 +958,31 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>1076</v>
+        <v>707</v>
       </c>
       <c r="D10">
-        <v>0.002263141563162208</v>
+        <v>0.001186518464237452</v>
       </c>
       <c r="E10">
-        <v>0.5300195119925775</v>
+        <v>0.2764706989983097</v>
       </c>
       <c r="F10">
-        <v>1076</v>
+        <v>707</v>
       </c>
       <c r="G10">
-        <v>0.03773193119559437</v>
+        <v>0.02072662871796638</v>
       </c>
       <c r="H10">
-        <v>0.2827433811617084</v>
+        <v>0.1732716474216431</v>
       </c>
       <c r="I10">
-        <v>0.04722965729888529</v>
+        <v>0.009598656557500362</v>
       </c>
       <c r="J10">
-        <v>0.1120653837569989</v>
+        <v>0.04189795663114637</v>
       </c>
       <c r="K10">
-        <v>0.01247106323717162</v>
+        <v>0.007737652049399912</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -991,10 +991,10 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>24025</v>
+        <v>4805</v>
       </c>
       <c r="E11">
-        <v>4.313439255172852</v>
+        <v>1.029153865994886</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1005,31 +1005,31 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>95</v>
+        <v>1823</v>
       </c>
       <c r="D12">
-        <v>0.01128185336710885</v>
+        <v>0.02205983060412109</v>
       </c>
       <c r="E12">
-        <v>0.108762368967291</v>
+        <v>0.726483765989542</v>
       </c>
       <c r="F12">
-        <v>95</v>
+        <v>1823</v>
       </c>
       <c r="G12">
-        <v>0.00400402897503227</v>
+        <v>0.0547923871781677</v>
       </c>
       <c r="H12">
-        <v>0.04074828908778727</v>
+        <v>0.4769193021347746</v>
       </c>
       <c r="I12">
-        <v>0.02542846312280744</v>
+        <v>0.03116031002718955</v>
       </c>
       <c r="J12">
-        <v>0.03382576227886602</v>
+        <v>0.08260764647275209</v>
       </c>
       <c r="K12">
-        <v>0.00121452403254807</v>
+        <v>0.02003651857376099</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1038,31 +1038,31 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>1139</v>
+        <v>855</v>
       </c>
       <c r="D13">
-        <v>0.001612934633158147</v>
+        <v>0.0008611893281340599</v>
       </c>
       <c r="E13">
-        <v>0.5421153209754266</v>
+        <v>0.3242480909684673</v>
       </c>
       <c r="F13">
-        <v>1139</v>
+        <v>855</v>
       </c>
       <c r="G13">
-        <v>0.04046279605245218</v>
+        <v>0.02528036874718964</v>
       </c>
       <c r="H13">
-        <v>0.2914333246299066</v>
+        <v>0.2062780619598925</v>
       </c>
       <c r="I13">
-        <v>0.04467568662948906</v>
+        <v>0.007863161503337324</v>
       </c>
       <c r="J13">
-        <v>0.1123796220635995</v>
+        <v>0.04654615197796375</v>
       </c>
       <c r="K13">
-        <v>0.01325282169273123</v>
+        <v>0.009509829105809331</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1071,31 +1071,31 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>95</v>
+        <v>855</v>
       </c>
       <c r="D14">
-        <v>0.01104365062201396</v>
+        <v>0.00881702231708914</v>
       </c>
       <c r="E14">
-        <v>0.1080448610009626</v>
+        <v>0.3386389480438083</v>
       </c>
       <c r="F14">
-        <v>95</v>
+        <v>855</v>
       </c>
       <c r="G14">
-        <v>0.003872684028465301</v>
+        <v>0.02580453595146537</v>
       </c>
       <c r="H14">
-        <v>0.03980063396738842</v>
+        <v>0.217749941861257</v>
       </c>
       <c r="I14">
-        <v>0.0252315869438462</v>
+        <v>0.009843258303590119</v>
       </c>
       <c r="J14">
-        <v>0.03434043121524155</v>
+        <v>0.04759739525616169</v>
       </c>
       <c r="K14">
-        <v>0.001204381347633898</v>
+        <v>0.009342187666334212</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1104,31 +1104,31 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>1139</v>
+        <v>855</v>
       </c>
       <c r="D15">
-        <v>0.002337873040232807</v>
+        <v>0.001334894681349397</v>
       </c>
       <c r="E15">
-        <v>0.5432634900207631</v>
+        <v>0.3278302811086178</v>
       </c>
       <c r="F15">
-        <v>1139</v>
+        <v>855</v>
       </c>
       <c r="G15">
-        <v>0.0393920264323242</v>
+        <v>0.02561569621320814</v>
       </c>
       <c r="H15">
-        <v>0.2918605352169834</v>
+        <v>0.2084406393114477</v>
       </c>
       <c r="I15">
-        <v>0.04816324287094176</v>
+        <v>0.008960254141129553</v>
       </c>
       <c r="J15">
-        <v>0.1121260161744431</v>
+        <v>0.04726952570490539</v>
       </c>
       <c r="K15">
-        <v>0.01299750007456169</v>
+        <v>0.009454978513531387</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1137,10 +1137,10 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>24025</v>
+        <v>4805</v>
       </c>
       <c r="E16">
-        <v>4.368436255026609</v>
+        <v>0.9926358649972826</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1151,31 +1151,31 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>109</v>
+        <v>1245</v>
       </c>
       <c r="D17">
-        <v>0.01047400326933712</v>
+        <v>0.01364321040455252</v>
       </c>
       <c r="E17">
-        <v>0.108120188000612</v>
+        <v>0.4918821790488437</v>
       </c>
       <c r="F17">
-        <v>109</v>
+        <v>1245</v>
       </c>
       <c r="G17">
-        <v>0.004190425155684352</v>
+        <v>0.03681550000328571</v>
       </c>
       <c r="H17">
-        <v>0.04230306309182197</v>
+        <v>0.3218109229346737</v>
       </c>
       <c r="I17">
-        <v>0.02306164166657254</v>
+        <v>0.02245280146598816</v>
       </c>
       <c r="J17">
-        <v>0.03341973992064595</v>
+        <v>0.0559447273844853</v>
       </c>
       <c r="K17">
-        <v>0.001318582973908633</v>
+        <v>0.01334235642571002</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1184,31 +1184,31 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>1109</v>
+        <v>591</v>
       </c>
       <c r="D18">
-        <v>0.001529842033050954</v>
+        <v>0.0006267315475270152</v>
       </c>
       <c r="E18">
-        <v>0.5266481360304169</v>
+        <v>0.2261388130718842</v>
       </c>
       <c r="F18">
-        <v>1109</v>
+        <v>591</v>
       </c>
       <c r="G18">
-        <v>0.0395005812169984</v>
+        <v>0.01741581899113953</v>
       </c>
       <c r="H18">
-        <v>0.2898613153374754</v>
+        <v>0.1438372770790011</v>
       </c>
       <c r="I18">
-        <v>0.03687580901896581</v>
+        <v>0.005481239408254623</v>
       </c>
       <c r="J18">
-        <v>0.1085626555723138</v>
+        <v>0.0332215492380783</v>
       </c>
       <c r="K18">
-        <v>0.01296313357306644</v>
+        <v>0.0064511300297454</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1217,31 +1217,31 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>109</v>
+        <v>591</v>
       </c>
       <c r="D19">
-        <v>0.01028783846413717</v>
+        <v>0.006310588214546442</v>
       </c>
       <c r="E19">
-        <v>0.1069873939850368</v>
+        <v>0.2399847289780155</v>
       </c>
       <c r="F19">
-        <v>109</v>
+        <v>591</v>
       </c>
       <c r="G19">
-        <v>0.004286327981390059</v>
+        <v>0.01770824962295592</v>
       </c>
       <c r="H19">
-        <v>0.04159283492481336</v>
+        <v>0.1552030059974641</v>
       </c>
       <c r="I19">
-        <v>0.0228524076519534</v>
+        <v>0.007016404648311436</v>
       </c>
       <c r="J19">
-        <v>0.03311938553815708</v>
+        <v>0.03406144538894296</v>
       </c>
       <c r="K19">
-        <v>0.001304226054344326</v>
+        <v>0.006488861632533371</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1250,31 +1250,31 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>1109</v>
+        <v>591</v>
       </c>
       <c r="D20">
-        <v>0.002247130672913045</v>
+        <v>0.0009861706057563424</v>
       </c>
       <c r="E20">
-        <v>0.5216129479813389</v>
+        <v>0.2281700660241768</v>
       </c>
       <c r="F20">
-        <v>1109</v>
+        <v>591</v>
       </c>
       <c r="G20">
-        <v>0.03855473216390237</v>
+        <v>0.01733138435520232</v>
       </c>
       <c r="H20">
-        <v>0.286038278893102</v>
+        <v>0.1450486677931622</v>
       </c>
       <c r="I20">
-        <v>0.04015162977157161</v>
+        <v>0.006312734563834965</v>
       </c>
       <c r="J20">
-        <v>0.1056350267026573</v>
+        <v>0.03404790908098221</v>
       </c>
       <c r="K20">
-        <v>0.01279978227103129</v>
+        <v>0.006336680613458157</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1283,10 +1283,10 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>24025</v>
+        <v>4805</v>
       </c>
       <c r="E21">
-        <v>4.54199444578262</v>
+        <v>1.202622185926884</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1297,31 +1297,31 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>82</v>
+        <v>2170</v>
       </c>
       <c r="D22">
-        <v>0.009767162497155368</v>
+        <v>0.02668864489533007</v>
       </c>
       <c r="E22">
-        <v>0.1014858980197459</v>
+        <v>0.8560476240236312</v>
       </c>
       <c r="F22">
-        <v>82</v>
+        <v>2170</v>
       </c>
       <c r="G22">
-        <v>0.003490472096018493</v>
+        <v>0.06420882721431553</v>
       </c>
       <c r="H22">
-        <v>0.03523752634646371</v>
+        <v>0.5605792781570926</v>
       </c>
       <c r="I22">
-        <v>0.0260842441348359</v>
+        <v>0.04085709701757878</v>
       </c>
       <c r="J22">
-        <v>0.03264433617005125</v>
+        <v>0.09624304971657693</v>
       </c>
       <c r="K22">
-        <v>0.001026042329613119</v>
+        <v>0.02330316929146647</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1330,31 +1330,31 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>1040</v>
+        <v>976</v>
       </c>
       <c r="D23">
-        <v>0.001425115158781409</v>
+        <v>0.0008980858838185668</v>
       </c>
       <c r="E23">
-        <v>0.4754166679922491</v>
+        <v>0.3461714800214395</v>
       </c>
       <c r="F23">
-        <v>1040</v>
+        <v>976</v>
       </c>
       <c r="G23">
-        <v>0.03548339934786782</v>
+        <v>0.02731961489189416</v>
       </c>
       <c r="H23">
-        <v>0.2556480597122572</v>
+        <v>0.2216545251430944</v>
       </c>
       <c r="I23">
-        <v>0.03934982267674059</v>
+        <v>0.009241797495633364</v>
       </c>
       <c r="J23">
-        <v>0.09885963768465444</v>
+        <v>0.04734734527301043</v>
       </c>
       <c r="K23">
-        <v>0.01149439241271466</v>
+        <v>0.01030507707037032</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1363,31 +1363,31 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>82</v>
+        <v>976</v>
       </c>
       <c r="D24">
-        <v>0.009940722782630473</v>
+        <v>0.01032575033605099</v>
       </c>
       <c r="E24">
-        <v>0.100390626990702</v>
+        <v>0.3793565769447014</v>
       </c>
       <c r="F24">
-        <v>82</v>
+        <v>976</v>
       </c>
       <c r="G24">
-        <v>0.003384889278095216</v>
+        <v>0.02844432753045112</v>
       </c>
       <c r="H24">
-        <v>0.03469320980366319</v>
+        <v>0.2465887044090778</v>
       </c>
       <c r="I24">
-        <v>0.02478584373602644</v>
+        <v>0.01109551044646651</v>
       </c>
       <c r="J24">
-        <v>0.03361548006068915</v>
+        <v>0.05100856814533472</v>
       </c>
       <c r="K24">
-        <v>0.0009879089775495231</v>
+        <v>0.01063325954601169</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1396,31 +1396,31 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>1040</v>
+        <v>976</v>
       </c>
       <c r="D25">
-        <v>0.002115348004736006</v>
+        <v>0.001531971851363778</v>
       </c>
       <c r="E25">
-        <v>0.4831616710289381</v>
+        <v>0.3688036509556696</v>
       </c>
       <c r="F25">
-        <v>1040</v>
+        <v>976</v>
       </c>
       <c r="G25">
-        <v>0.03499974741134793</v>
+        <v>0.02935354050714523</v>
       </c>
       <c r="H25">
-        <v>0.2572847756673582</v>
+        <v>0.2364394528558478</v>
       </c>
       <c r="I25">
-        <v>0.04348528449190781</v>
+        <v>0.01073132548481226</v>
       </c>
       <c r="J25">
-        <v>0.101119686733</v>
+        <v>0.05059266509488225</v>
       </c>
       <c r="K25">
-        <v>0.01155237737111747</v>
+        <v>0.01033912471029907</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1429,10 +1429,10 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>24025</v>
+        <v>4805</v>
       </c>
       <c r="E26">
-        <v>4.58458932407666</v>
+        <v>0.841553280246444</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1443,31 +1443,31 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>92.59999999999999</v>
+        <v>1728.2</v>
       </c>
       <c r="D27">
-        <v>0.01016216996358708</v>
+        <v>0.02076922613196075</v>
       </c>
       <c r="E27">
-        <v>0.1030309191904962</v>
+        <v>0.6913670442067087</v>
       </c>
       <c r="F27">
-        <v>92.59999999999999</v>
+        <v>1728.2</v>
       </c>
       <c r="G27">
-        <v>0.003731282206717879</v>
+        <v>0.05174948906060308</v>
       </c>
       <c r="H27">
-        <v>0.03799828748451546</v>
+        <v>0.4528925512684509</v>
       </c>
       <c r="I27">
-        <v>0.0239810582017526</v>
+        <v>0.03217250595334917</v>
       </c>
       <c r="J27">
-        <v>0.03289601246360689</v>
+        <v>0.07827201758045703</v>
       </c>
       <c r="K27">
-        <v>0.001143887068610638</v>
+        <v>0.01880766048561782</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1476,31 +1476,31 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>1064</v>
+        <v>799</v>
       </c>
       <c r="D28">
-        <v>0.00150680715451017</v>
+        <v>0.0008129928028210998</v>
       </c>
       <c r="E28">
-        <v>0.5066931535955519</v>
+        <v>0.2994565485976636</v>
       </c>
       <c r="F28">
-        <v>1064</v>
+        <v>799</v>
       </c>
       <c r="G28">
-        <v>0.0376589416526258</v>
+        <v>0.02316260437946767</v>
       </c>
       <c r="H28">
-        <v>0.2743025582749397</v>
+        <v>0.1910222575301304</v>
       </c>
       <c r="I28">
-        <v>0.04005886344239116</v>
+        <v>0.007689380878582596</v>
       </c>
       <c r="J28">
-        <v>0.1052897942950949</v>
+        <v>0.04297278716694564</v>
       </c>
       <c r="K28">
-        <v>0.01233727465150878</v>
+        <v>0.00863105517346412</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1509,31 +1509,31 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>92.8</v>
+        <v>799</v>
       </c>
       <c r="D29">
-        <v>0.01013298451434821</v>
+        <v>0.00906791421584785</v>
       </c>
       <c r="E29">
-        <v>0.102303409203887</v>
+        <v>0.327202022401616</v>
       </c>
       <c r="F29">
-        <v>92.8</v>
+        <v>799</v>
       </c>
       <c r="G29">
-        <v>0.003692255145870149</v>
+        <v>0.02445398936979472</v>
       </c>
       <c r="H29">
-        <v>0.0374988014344126</v>
+        <v>0.2111626660684124</v>
       </c>
       <c r="I29">
-        <v>0.02365071171661839</v>
+        <v>0.009911233256570996</v>
       </c>
       <c r="J29">
-        <v>0.03306425634073094</v>
+        <v>0.04573364946991205</v>
       </c>
       <c r="K29">
-        <v>0.001123691257089376</v>
+        <v>0.00898289680480957</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1542,31 +1542,31 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>1064</v>
+        <v>799</v>
       </c>
       <c r="D30">
-        <v>0.002202699135523289</v>
+        <v>0.001286801532842219</v>
       </c>
       <c r="E30">
-        <v>0.5072409691987559</v>
+        <v>0.3071046628290787</v>
       </c>
       <c r="F30">
-        <v>1064</v>
+        <v>799</v>
       </c>
       <c r="G30">
-        <v>0.03682333879405632</v>
+        <v>0.02382008000276983</v>
       </c>
       <c r="H30">
-        <v>0.2729375449474901</v>
+        <v>0.1953356698388234</v>
       </c>
       <c r="I30">
-        <v>0.04374331606086344</v>
+        <v>0.008897774410434068</v>
       </c>
       <c r="J30">
-        <v>0.1050166505621746</v>
+        <v>0.044248784519732</v>
       </c>
       <c r="K30">
-        <v>0.01216060154838488</v>
+        <v>0.008709695236757398</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1575,10 +1575,10 @@
         <v>25</v>
       </c>
       <c r="C31">
-        <v>24025</v>
+        <v>4805</v>
       </c>
       <c r="E31">
-        <v>4.469126798806246</v>
+        <v>1.006955873873085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unmerged can meet somewhere in the middle now
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -716,28 +716,28 @@
         <v>1840</v>
       </c>
       <c r="D2">
-        <v>0.02247039030771703</v>
+        <v>0.03132899571210146</v>
       </c>
       <c r="E2">
-        <v>0.7443019769852981</v>
+        <v>0.8465258019277826</v>
       </c>
       <c r="F2">
         <v>1840</v>
       </c>
       <c r="G2">
-        <v>0.05537386040668935</v>
+        <v>0.06328552949707955</v>
       </c>
       <c r="H2">
-        <v>0.4904221027391031</v>
+        <v>0.5563925282331184</v>
       </c>
       <c r="I2">
-        <v>0.03413118747994304</v>
+        <v>0.0363466510316357</v>
       </c>
       <c r="J2">
-        <v>0.08356877986807376</v>
+        <v>0.09707645187154412</v>
       </c>
       <c r="K2">
-        <v>0.01999597204849124</v>
+        <v>0.02347082155756652</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -746,31 +746,31 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>866</v>
+        <v>715</v>
       </c>
       <c r="D3">
-        <v>0.0009043698664754629</v>
+        <v>0.0007684332085773349</v>
       </c>
       <c r="E3">
-        <v>0.3264306769706309</v>
+        <v>0.2694176440127194</v>
       </c>
       <c r="F3">
-        <v>866</v>
+        <v>715</v>
       </c>
       <c r="G3">
-        <v>0.02500208560377359</v>
+        <v>0.02111801982391626</v>
       </c>
       <c r="H3">
-        <v>0.2106004991801456</v>
+        <v>0.1761669169645756</v>
       </c>
       <c r="I3">
-        <v>0.007719359477050602</v>
+        <v>0.006703459774143994</v>
       </c>
       <c r="J3">
-        <v>0.04627484793309122</v>
+        <v>0.03396003588568419</v>
       </c>
       <c r="K3">
-        <v>0.009199967258609831</v>
+        <v>0.007764974609017372</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -779,31 +779,31 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>866</v>
+        <v>715</v>
       </c>
       <c r="D4">
-        <v>0.009958986309356987</v>
+        <v>0.01371360733173788</v>
       </c>
       <c r="E4">
-        <v>0.3579659190727398</v>
+        <v>0.3480011560022831</v>
       </c>
       <c r="F4">
-        <v>866</v>
+        <v>715</v>
       </c>
       <c r="G4">
-        <v>0.02703198709059507</v>
+        <v>0.02644675597548485</v>
       </c>
       <c r="H4">
-        <v>0.2321864258265123</v>
+        <v>0.2291291250148788</v>
       </c>
       <c r="I4">
-        <v>0.009908543550409377</v>
+        <v>0.009758537402376533</v>
       </c>
       <c r="J4">
-        <v>0.04946563148405403</v>
+        <v>0.04374468501191586</v>
       </c>
       <c r="K4">
-        <v>0.009843050269410014</v>
+        <v>0.009559829370118678</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -812,31 +812,31 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>866</v>
+        <v>715</v>
       </c>
       <c r="D5">
-        <v>0.001394452061504126</v>
+        <v>0.001299587893299758</v>
       </c>
       <c r="E5">
-        <v>0.3342486170586199</v>
+        <v>0.3111274240072817</v>
       </c>
       <c r="F5">
-        <v>866</v>
+        <v>715</v>
       </c>
       <c r="G5">
-        <v>0.02607315022032708</v>
+        <v>0.02459960756823421</v>
       </c>
       <c r="H5">
-        <v>0.2134779418120161</v>
+        <v>0.2021545793395489</v>
       </c>
       <c r="I5">
-        <v>0.008885901304893196</v>
+        <v>0.009164535324089229</v>
       </c>
       <c r="J5">
-        <v>0.04743586608674377</v>
+        <v>0.03857860108837485</v>
       </c>
       <c r="K5">
-        <v>0.009680040297098458</v>
+        <v>0.009044826379977167</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -848,7 +848,7 @@
         <v>4805</v>
       </c>
       <c r="E6">
-        <v>0.9688141721999273</v>
+        <v>1.07732873596251</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -862,28 +862,28 @@
         <v>1563</v>
       </c>
       <c r="D7">
-        <v>0.01898405444808304</v>
+        <v>0.02745914075057954</v>
       </c>
       <c r="E7">
-        <v>0.6381196749862283</v>
+        <v>0.7452965029515326</v>
       </c>
       <c r="F7">
         <v>1563</v>
       </c>
       <c r="G7">
-        <v>0.04755687050055712</v>
+        <v>0.05512112902943045</v>
       </c>
       <c r="H7">
-        <v>0.4147311503766105</v>
+        <v>0.488878053962253</v>
       </c>
       <c r="I7">
-        <v>0.03226113377604634</v>
+        <v>0.03434200666379184</v>
       </c>
       <c r="J7">
-        <v>0.07299588446039706</v>
+        <v>0.0852981461212039</v>
       </c>
       <c r="K7">
-        <v>0.01736028608866036</v>
+        <v>0.02053049392998219</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -892,31 +892,31 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>707</v>
+        <v>518</v>
       </c>
       <c r="D8">
-        <v>0.000774587388150394</v>
+        <v>0.0006273738108575344</v>
       </c>
       <c r="E8">
-        <v>0.2742936819558963</v>
+        <v>0.2022015820257366</v>
       </c>
       <c r="F8">
-        <v>707</v>
+        <v>518</v>
       </c>
       <c r="G8">
-        <v>0.0207951336633414</v>
+        <v>0.01577108656056225</v>
       </c>
       <c r="H8">
-        <v>0.1727409242885187</v>
+        <v>0.1308854530798271</v>
       </c>
       <c r="I8">
-        <v>0.008141346508637071</v>
+        <v>0.006195415859110653</v>
       </c>
       <c r="J8">
-        <v>0.04147404141258448</v>
+        <v>0.02601894538383931</v>
       </c>
       <c r="K8">
-        <v>0.007689272402785718</v>
+        <v>0.005786096910014749</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -925,31 +925,31 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>707</v>
+        <v>518</v>
       </c>
       <c r="D9">
-        <v>0.009927223902195692</v>
+        <v>0.01210114860441536</v>
       </c>
       <c r="E9">
-        <v>0.3200639389688149</v>
+        <v>0.2791609010891989</v>
       </c>
       <c r="F9">
-        <v>707</v>
+        <v>518</v>
       </c>
       <c r="G9">
-        <v>0.02328084665350616</v>
+        <v>0.02025187818799168</v>
       </c>
       <c r="H9">
-        <v>0.2040852522477508</v>
+        <v>0.1845295174280182</v>
       </c>
       <c r="I9">
-        <v>0.01169244933407754</v>
+        <v>0.009838219033554196</v>
       </c>
       <c r="J9">
-        <v>0.04653520707506686</v>
+        <v>0.03408847749233246</v>
       </c>
       <c r="K9">
-        <v>0.008607124909758568</v>
+        <v>0.007446028175763786</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -958,31 +958,31 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>707</v>
+        <v>518</v>
       </c>
       <c r="D10">
-        <v>0.001186518464237452</v>
+        <v>0.0009174455190077424</v>
       </c>
       <c r="E10">
-        <v>0.2764706989983097</v>
+        <v>0.2039270030800253</v>
       </c>
       <c r="F10">
-        <v>707</v>
+        <v>518</v>
       </c>
       <c r="G10">
-        <v>0.02072662871796638</v>
+        <v>0.01543852221220732</v>
       </c>
       <c r="H10">
-        <v>0.1732716474216431</v>
+        <v>0.1317497495329008</v>
       </c>
       <c r="I10">
-        <v>0.009598656557500362</v>
+        <v>0.007365834666416049</v>
       </c>
       <c r="J10">
-        <v>0.04189795663114637</v>
+        <v>0.02613346138969064</v>
       </c>
       <c r="K10">
-        <v>0.007737652049399912</v>
+        <v>0.005712611950002611</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -994,7 +994,7 @@
         <v>4805</v>
       </c>
       <c r="E11">
-        <v>1.029153865994886</v>
+        <v>0.883647444890812</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1008,28 +1008,28 @@
         <v>1823</v>
       </c>
       <c r="D12">
-        <v>0.02205983060412109</v>
+        <v>0.03061900229658931</v>
       </c>
       <c r="E12">
-        <v>0.726483765989542</v>
+        <v>0.8513227259973064</v>
       </c>
       <c r="F12">
         <v>1823</v>
       </c>
       <c r="G12">
-        <v>0.0547923871781677</v>
+        <v>0.06384283024817705</v>
       </c>
       <c r="H12">
-        <v>0.4769193021347746</v>
+        <v>0.5600891294889152</v>
       </c>
       <c r="I12">
-        <v>0.03116031002718955</v>
+        <v>0.03298931068275124</v>
       </c>
       <c r="J12">
-        <v>0.08260764647275209</v>
+        <v>0.09828316757921129</v>
       </c>
       <c r="K12">
-        <v>0.02003651857376099</v>
+        <v>0.02422631497029215</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1038,31 +1038,31 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>855</v>
+        <v>730</v>
       </c>
       <c r="D13">
-        <v>0.0008611893281340599</v>
+        <v>0.0007934162858873606</v>
       </c>
       <c r="E13">
-        <v>0.3242480909684673</v>
+        <v>0.2836754629388452</v>
       </c>
       <c r="F13">
-        <v>855</v>
+        <v>730</v>
       </c>
       <c r="G13">
-        <v>0.02528036874718964</v>
+        <v>0.0223809196613729</v>
       </c>
       <c r="H13">
-        <v>0.2062780619598925</v>
+        <v>0.1851774787064642</v>
       </c>
       <c r="I13">
-        <v>0.007863161503337324</v>
+        <v>0.007017820025794208</v>
       </c>
       <c r="J13">
-        <v>0.04654615197796375</v>
+        <v>0.03524050302803516</v>
       </c>
       <c r="K13">
-        <v>0.009509829105809331</v>
+        <v>0.008320488268509507</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1071,31 +1071,31 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>855</v>
+        <v>730</v>
       </c>
       <c r="D14">
-        <v>0.00881702231708914</v>
+        <v>0.01028321927879006</v>
       </c>
       <c r="E14">
-        <v>0.3386389480438083</v>
+        <v>0.3006821880117059</v>
       </c>
       <c r="F14">
-        <v>855</v>
+        <v>730</v>
       </c>
       <c r="G14">
-        <v>0.02580453595146537</v>
+        <v>0.02312570333015174</v>
       </c>
       <c r="H14">
-        <v>0.217749941861257</v>
+        <v>0.1983913854928687</v>
       </c>
       <c r="I14">
-        <v>0.009843258303590119</v>
+        <v>0.008141801808960736</v>
       </c>
       <c r="J14">
-        <v>0.04759739525616169</v>
+        <v>0.03662345535121858</v>
       </c>
       <c r="K14">
-        <v>0.009342187666334212</v>
+        <v>0.008495513233356178</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1104,31 +1104,31 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>855</v>
+        <v>730</v>
       </c>
       <c r="D15">
-        <v>0.001334894681349397</v>
+        <v>0.001296792179346085</v>
       </c>
       <c r="E15">
-        <v>0.3278302811086178</v>
+        <v>0.3124301059870049</v>
       </c>
       <c r="F15">
-        <v>855</v>
+        <v>730</v>
       </c>
       <c r="G15">
-        <v>0.02561569621320814</v>
+        <v>0.02493431628681719</v>
       </c>
       <c r="H15">
-        <v>0.2084406393114477</v>
+        <v>0.2024387046694756</v>
       </c>
       <c r="I15">
-        <v>0.008960254141129553</v>
+        <v>0.009120996575802565</v>
       </c>
       <c r="J15">
-        <v>0.04726952570490539</v>
+        <v>0.03920478466898203</v>
       </c>
       <c r="K15">
-        <v>0.009454978513531387</v>
+        <v>0.009039454045705497</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1140,7 +1140,7 @@
         <v>4805</v>
       </c>
       <c r="E16">
-        <v>0.9926358649972826</v>
+        <v>1.009621520992368</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1154,28 +1154,28 @@
         <v>1245</v>
       </c>
       <c r="D17">
-        <v>0.01364321040455252</v>
+        <v>0.01865265902597457</v>
       </c>
       <c r="E17">
-        <v>0.4918821790488437</v>
+        <v>0.5483171029482037</v>
       </c>
       <c r="F17">
         <v>1245</v>
       </c>
       <c r="G17">
-        <v>0.03681550000328571</v>
+        <v>0.04096021328587085</v>
       </c>
       <c r="H17">
-        <v>0.3218109229346737</v>
+        <v>0.3597754908259958</v>
       </c>
       <c r="I17">
-        <v>0.02245280146598816</v>
+        <v>0.02196197852026671</v>
       </c>
       <c r="J17">
-        <v>0.0559447273844853</v>
+        <v>0.06441310828085989</v>
       </c>
       <c r="K17">
-        <v>0.01334235642571002</v>
+        <v>0.01543511194176972</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1184,31 +1184,31 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>591</v>
+        <v>455</v>
       </c>
       <c r="D18">
-        <v>0.0006267315475270152</v>
+        <v>0.0005149961216375232</v>
       </c>
       <c r="E18">
-        <v>0.2261388130718842</v>
+        <v>0.1739185689948499</v>
       </c>
       <c r="F18">
-        <v>591</v>
+        <v>455</v>
       </c>
       <c r="G18">
-        <v>0.01741581899113953</v>
+        <v>0.01389433315489441</v>
       </c>
       <c r="H18">
-        <v>0.1438372770790011</v>
+        <v>0.1133973768446594</v>
       </c>
       <c r="I18">
-        <v>0.005481239408254623</v>
+        <v>0.004485916229896247</v>
       </c>
       <c r="J18">
-        <v>0.0332215492380783</v>
+        <v>0.02178795787040144</v>
       </c>
       <c r="K18">
-        <v>0.0064511300297454</v>
+        <v>0.005020585376769304</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1217,31 +1217,31 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>591</v>
+        <v>455</v>
       </c>
       <c r="D19">
-        <v>0.006310588214546442</v>
+        <v>0.008697166456840932</v>
       </c>
       <c r="E19">
-        <v>0.2399847289780155</v>
+        <v>0.2488408359931782</v>
       </c>
       <c r="F19">
-        <v>591</v>
+        <v>455</v>
       </c>
       <c r="G19">
-        <v>0.01770824962295592</v>
+        <v>0.0189931420609355</v>
       </c>
       <c r="H19">
-        <v>0.1552030059974641</v>
+        <v>0.1638728112448007</v>
       </c>
       <c r="I19">
-        <v>0.007016404648311436</v>
+        <v>0.006947503890842199</v>
       </c>
       <c r="J19">
-        <v>0.03406144538894296</v>
+        <v>0.03112816507928073</v>
       </c>
       <c r="K19">
-        <v>0.006488861632533371</v>
+        <v>0.006911113508976996</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1250,31 +1250,31 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>591</v>
+        <v>455</v>
       </c>
       <c r="D20">
-        <v>0.0009861706057563424</v>
+        <v>0.0007867485983297229</v>
       </c>
       <c r="E20">
-        <v>0.2281700660241768</v>
+        <v>0.1742072280030698</v>
       </c>
       <c r="F20">
-        <v>591</v>
+        <v>455</v>
       </c>
       <c r="G20">
-        <v>0.01733138435520232</v>
+        <v>0.01360937999561429</v>
       </c>
       <c r="H20">
-        <v>0.1450486677931622</v>
+        <v>0.1127434713998809</v>
       </c>
       <c r="I20">
-        <v>0.006312734563834965</v>
+        <v>0.005213191383518279</v>
       </c>
       <c r="J20">
-        <v>0.03404790908098221</v>
+        <v>0.02255417127162218</v>
       </c>
       <c r="K20">
-        <v>0.006336680613458157</v>
+        <v>0.004959819838404655</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1286,7 +1286,7 @@
         <v>4805</v>
       </c>
       <c r="E21">
-        <v>1.202622185926884</v>
+        <v>0.9897040039068088</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1297,31 +1297,31 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="D22">
-        <v>0.02668864489533007</v>
+        <v>0.03284667024854571</v>
       </c>
       <c r="E22">
-        <v>0.8560476240236312</v>
+        <v>0.8966879429062828</v>
       </c>
       <c r="F22">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="G22">
-        <v>0.06420882721431553</v>
+        <v>0.06800082640256733</v>
       </c>
       <c r="H22">
-        <v>0.5605792781570926</v>
+        <v>0.5866953654913232</v>
       </c>
       <c r="I22">
-        <v>0.04085709701757878</v>
+        <v>0.03994058596435934</v>
       </c>
       <c r="J22">
-        <v>0.09624304971657693</v>
+        <v>0.1019669460365549</v>
       </c>
       <c r="K22">
-        <v>0.02330316929146647</v>
+        <v>0.02500429155770689</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1330,31 +1330,31 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>976</v>
+        <v>844</v>
       </c>
       <c r="D23">
-        <v>0.0008980858838185668</v>
+        <v>0.000826406991109252</v>
       </c>
       <c r="E23">
-        <v>0.3461714800214395</v>
+        <v>0.2956173539860174</v>
       </c>
       <c r="F23">
-        <v>976</v>
+        <v>844</v>
       </c>
       <c r="G23">
-        <v>0.02731961489189416</v>
+        <v>0.02358393406029791</v>
       </c>
       <c r="H23">
-        <v>0.2216545251430944</v>
+        <v>0.1913351627299562</v>
       </c>
       <c r="I23">
-        <v>0.009241797495633364</v>
+        <v>0.007521819206885993</v>
       </c>
       <c r="J23">
-        <v>0.04734734527301043</v>
+        <v>0.03799583250656724</v>
       </c>
       <c r="K23">
-        <v>0.01030507707037032</v>
+        <v>0.008596397819928825</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1363,31 +1363,31 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>976</v>
+        <v>844</v>
       </c>
       <c r="D24">
-        <v>0.01032575033605099</v>
+        <v>0.01128954836167395</v>
       </c>
       <c r="E24">
-        <v>0.3793565769447014</v>
+        <v>0.3228164649335667</v>
       </c>
       <c r="F24">
-        <v>976</v>
+        <v>844</v>
       </c>
       <c r="G24">
-        <v>0.02844432753045112</v>
+        <v>0.02452081348747015</v>
       </c>
       <c r="H24">
-        <v>0.2465887044090778</v>
+        <v>0.2126501726452261</v>
       </c>
       <c r="I24">
-        <v>0.01109551044646651</v>
+        <v>0.009120725793763995</v>
       </c>
       <c r="J24">
-        <v>0.05100856814533472</v>
+        <v>0.03968897426966578</v>
       </c>
       <c r="K24">
-        <v>0.01063325954601169</v>
+        <v>0.009195050457492471</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1396,31 +1396,31 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>976</v>
+        <v>844</v>
       </c>
       <c r="D25">
-        <v>0.001531971851363778</v>
+        <v>0.001329442718997598</v>
       </c>
       <c r="E25">
-        <v>0.3688036509556696</v>
+        <v>0.3160389759577811</v>
       </c>
       <c r="F25">
-        <v>976</v>
+        <v>844</v>
       </c>
       <c r="G25">
-        <v>0.02935354050714523</v>
+        <v>0.02509266068227589</v>
       </c>
       <c r="H25">
-        <v>0.2364394528558478</v>
+        <v>0.2045535693177953</v>
       </c>
       <c r="I25">
-        <v>0.01073132548481226</v>
+        <v>0.009361646138131618</v>
       </c>
       <c r="J25">
-        <v>0.05059266509488225</v>
+        <v>0.0400876043131575</v>
       </c>
       <c r="K25">
-        <v>0.01033912471029907</v>
+        <v>0.009019757620990276</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1432,7 +1432,7 @@
         <v>4805</v>
       </c>
       <c r="E26">
-        <v>0.841553280246444</v>
+        <v>0.870586880017072</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1443,31 +1443,31 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1728.2</v>
+        <v>1728</v>
       </c>
       <c r="D27">
-        <v>0.02076922613196075</v>
+        <v>0.02818129360675812</v>
       </c>
       <c r="E27">
-        <v>0.6913670442067087</v>
+        <v>0.7776300153462217</v>
       </c>
       <c r="F27">
-        <v>1728.2</v>
+        <v>1728</v>
       </c>
       <c r="G27">
-        <v>0.05174948906060308</v>
+        <v>0.05824210569262504</v>
       </c>
       <c r="H27">
-        <v>0.4528925512684509</v>
+        <v>0.5103661136003211</v>
       </c>
       <c r="I27">
-        <v>0.03217250595334917</v>
+        <v>0.03311610657256096</v>
       </c>
       <c r="J27">
-        <v>0.07827201758045703</v>
+        <v>0.08940756397787482</v>
       </c>
       <c r="K27">
-        <v>0.01880766048561782</v>
+        <v>0.0217334067914635</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1476,31 +1476,31 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>799</v>
+        <v>652.4</v>
       </c>
       <c r="D28">
-        <v>0.0008129928028210998</v>
+        <v>0.000706125283613801</v>
       </c>
       <c r="E28">
-        <v>0.2994565485976636</v>
+        <v>0.2449661223916337</v>
       </c>
       <c r="F28">
-        <v>799</v>
+        <v>652.4</v>
       </c>
       <c r="G28">
-        <v>0.02316260437946767</v>
+        <v>0.01934965865220874</v>
       </c>
       <c r="H28">
-        <v>0.1910222575301304</v>
+        <v>0.1593924776650965</v>
       </c>
       <c r="I28">
-        <v>0.007689380878582596</v>
+        <v>0.006384886219166219</v>
       </c>
       <c r="J28">
-        <v>0.04297278716694564</v>
+        <v>0.03100065493490547</v>
       </c>
       <c r="K28">
-        <v>0.00863105517346412</v>
+        <v>0.007097708596847952</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1509,31 +1509,31 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>799</v>
+        <v>652.4</v>
       </c>
       <c r="D29">
-        <v>0.00906791421584785</v>
+        <v>0.01121693800669163</v>
       </c>
       <c r="E29">
-        <v>0.327202022401616</v>
+        <v>0.2999003092059865</v>
       </c>
       <c r="F29">
-        <v>799</v>
+        <v>652.4</v>
       </c>
       <c r="G29">
-        <v>0.02445398936979472</v>
+        <v>0.02266765860840678</v>
       </c>
       <c r="H29">
-        <v>0.2111626660684124</v>
+        <v>0.1977146023651585</v>
       </c>
       <c r="I29">
-        <v>0.009911233256570996</v>
+        <v>0.008761357585899531</v>
       </c>
       <c r="J29">
-        <v>0.04573364946991205</v>
+        <v>0.03705475144088268</v>
       </c>
       <c r="K29">
-        <v>0.00898289680480957</v>
+        <v>0.008321506949141622</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1542,31 +1542,31 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>799</v>
+        <v>652.4</v>
       </c>
       <c r="D30">
-        <v>0.001286801532842219</v>
+        <v>0.001126003381796181</v>
       </c>
       <c r="E30">
-        <v>0.3071046628290787</v>
+        <v>0.2635461474070325</v>
       </c>
       <c r="F30">
-        <v>799</v>
+        <v>652.4</v>
       </c>
       <c r="G30">
-        <v>0.02382008000276983</v>
+        <v>0.02073489734902978</v>
       </c>
       <c r="H30">
-        <v>0.1953356698388234</v>
+        <v>0.1707280148519203</v>
       </c>
       <c r="I30">
-        <v>0.008897774410434068</v>
+        <v>0.008045240817591549</v>
       </c>
       <c r="J30">
-        <v>0.044248784519732</v>
+        <v>0.03331172454636544</v>
       </c>
       <c r="K30">
-        <v>0.008709695236757398</v>
+        <v>0.007555293967016041</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1578,7 +1578,7 @@
         <v>4805</v>
       </c>
       <c r="E31">
-        <v>1.006955873873085</v>
+        <v>0.9661777171539143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exposed Custom_Heuristics in common module, setUp and tearDown for some unit tests; unmerged doesn't pass test_run_heuristics
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -493,22 +493,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>59.452</v>
+        <v>41.48399999999999</v>
       </c>
       <c r="C2">
-        <v>50.59199999999999</v>
+        <v>61.694</v>
       </c>
       <c r="D2">
-        <v>50.59199999999999</v>
+        <v>61.694</v>
       </c>
       <c r="E2">
-        <v>50.59199999999999</v>
+        <v>61.694</v>
       </c>
       <c r="F2">
-        <v>50.59199999999999</v>
+        <v>61.694</v>
       </c>
       <c r="G2">
-        <v>0.1192222296979077</v>
+        <v>0.3897406228907532</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -528,22 +528,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>20.726</v>
+        <v>32.656</v>
       </c>
       <c r="C3">
-        <v>42.038</v>
+        <v>47.382</v>
       </c>
       <c r="D3">
-        <v>42.038</v>
+        <v>47.382</v>
       </c>
       <c r="E3">
-        <v>42.038</v>
+        <v>47.382</v>
       </c>
       <c r="F3">
-        <v>42.038</v>
+        <v>47.382</v>
       </c>
       <c r="G3">
-        <v>0.8226189327414839</v>
+        <v>0.3607545320921117</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -563,22 +563,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61.796</v>
+        <v>33.48399999999999</v>
       </c>
       <c r="C4">
-        <v>54.55399999999999</v>
+        <v>41.382</v>
       </c>
       <c r="D4">
-        <v>54.554</v>
+        <v>41.382</v>
       </c>
       <c r="E4">
-        <v>54.554</v>
+        <v>41.382</v>
       </c>
       <c r="F4">
-        <v>54.554</v>
+        <v>41.382</v>
       </c>
       <c r="G4">
-        <v>0.09375364101236328</v>
+        <v>0.1886990801576875</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -598,22 +598,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>40.108</v>
+        <v>50.038</v>
       </c>
       <c r="C5">
-        <v>37.14</v>
+        <v>48.20999999999999</v>
       </c>
       <c r="D5">
-        <v>37.14</v>
+        <v>48.20999999999999</v>
       </c>
       <c r="E5">
-        <v>37.14</v>
+        <v>48.20999999999999</v>
       </c>
       <c r="F5">
-        <v>37.14</v>
+        <v>48.20999999999999</v>
       </c>
       <c r="G5">
-        <v>0.05920015956916314</v>
+        <v>0.02922578840081569</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -633,22 +633,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>41.554</v>
+        <v>41.694</v>
       </c>
       <c r="C6">
-        <v>65.79599999999999</v>
+        <v>45.452</v>
       </c>
       <c r="D6">
-        <v>65.79599999999999</v>
+        <v>45.452</v>
       </c>
       <c r="E6">
-        <v>65.79599999999999</v>
+        <v>45.452</v>
       </c>
       <c r="F6">
-        <v>65.79599999999999</v>
+        <v>45.452</v>
       </c>
       <c r="G6">
-        <v>0.4667083794580542</v>
+        <v>0.07210629826833603</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -713,31 +713,31 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1840</v>
+        <v>103</v>
       </c>
       <c r="D2">
-        <v>0.03132899571210146</v>
+        <v>0.008189005544409156</v>
       </c>
       <c r="E2">
-        <v>0.8465258019277826</v>
+        <v>0.105924578034319</v>
       </c>
       <c r="F2">
-        <v>1840</v>
+        <v>103</v>
       </c>
       <c r="G2">
-        <v>0.06328552949707955</v>
+        <v>0.005882885656319559</v>
       </c>
       <c r="H2">
-        <v>0.5563925282331184</v>
+        <v>0.06969061761628836</v>
       </c>
       <c r="I2">
-        <v>0.0363466510316357</v>
+        <v>0.005414729355834424</v>
       </c>
       <c r="J2">
-        <v>0.09707645187154412</v>
+        <v>0.01658011670224369</v>
       </c>
       <c r="K2">
-        <v>0.02347082155756652</v>
+        <v>0.002096734941005707</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -746,31 +746,31 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>715</v>
+        <v>841</v>
       </c>
       <c r="D3">
-        <v>0.0007684332085773349</v>
+        <v>0.001355051877908409</v>
       </c>
       <c r="E3">
-        <v>0.2694176440127194</v>
+        <v>0.4458491399418563</v>
       </c>
       <c r="F3">
-        <v>715</v>
+        <v>841</v>
       </c>
       <c r="G3">
-        <v>0.02111801982391626</v>
+        <v>0.03444239869713783</v>
       </c>
       <c r="H3">
-        <v>0.1761669169645756</v>
+        <v>0.2877437327988446</v>
       </c>
       <c r="I3">
-        <v>0.006703459774143994</v>
+        <v>0.0161881810054183</v>
       </c>
       <c r="J3">
-        <v>0.03396003588568419</v>
+        <v>0.0571952520404011</v>
       </c>
       <c r="K3">
-        <v>0.007764974609017372</v>
+        <v>0.01244004664476961</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -779,31 +779,31 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>715</v>
+        <v>103</v>
       </c>
       <c r="D4">
-        <v>0.01371360733173788</v>
+        <v>0.005695371772162616</v>
       </c>
       <c r="E4">
-        <v>0.3480011560022831</v>
+        <v>0.1002145250095055</v>
       </c>
       <c r="F4">
-        <v>715</v>
+        <v>103</v>
       </c>
       <c r="G4">
-        <v>0.02644675597548485</v>
+        <v>0.01339302223641425</v>
       </c>
       <c r="H4">
-        <v>0.2291291250148788</v>
+        <v>0.06159640965051949</v>
       </c>
       <c r="I4">
-        <v>0.009758537402376533</v>
+        <v>0.001973273698240519</v>
       </c>
       <c r="J4">
-        <v>0.04374468501191586</v>
+        <v>0.01416924560908228</v>
       </c>
       <c r="K4">
-        <v>0.009559829370118678</v>
+        <v>0.002171794883906841</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -812,31 +812,31 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>715</v>
+        <v>841</v>
       </c>
       <c r="D5">
-        <v>0.001299587893299758</v>
+        <v>0.001980427536182106</v>
       </c>
       <c r="E5">
-        <v>0.3111274240072817</v>
+        <v>0.4499561260454357</v>
       </c>
       <c r="F5">
-        <v>715</v>
+        <v>841</v>
       </c>
       <c r="G5">
-        <v>0.02459960756823421</v>
+        <v>0.03585337020922452</v>
       </c>
       <c r="H5">
-        <v>0.2021545793395489</v>
+        <v>0.2926456088898703</v>
       </c>
       <c r="I5">
-        <v>0.009164535324089229</v>
+        <v>0.01467407483141869</v>
       </c>
       <c r="J5">
-        <v>0.03857860108837485</v>
+        <v>0.05429538327734917</v>
       </c>
       <c r="K5">
-        <v>0.009044826379977167</v>
+        <v>0.01307916862424463</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -848,7 +848,7 @@
         <v>4805</v>
       </c>
       <c r="E6">
-        <v>1.07732873596251</v>
+        <v>1.062308883643709</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -859,31 +859,31 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1563</v>
+        <v>59</v>
       </c>
       <c r="D7">
-        <v>0.02745914075057954</v>
+        <v>0.003549611894413829</v>
       </c>
       <c r="E7">
-        <v>0.7452965029515326</v>
+        <v>0.0703013630118221</v>
       </c>
       <c r="F7">
-        <v>1563</v>
+        <v>59</v>
       </c>
       <c r="G7">
-        <v>0.05512112902943045</v>
+        <v>0.003958272864110768</v>
       </c>
       <c r="H7">
-        <v>0.488878053962253</v>
+        <v>0.05023069749586284</v>
       </c>
       <c r="I7">
-        <v>0.03434200666379184</v>
+        <v>0.001357558649033308</v>
       </c>
       <c r="J7">
-        <v>0.0852981461212039</v>
+        <v>0.009682819480076432</v>
       </c>
       <c r="K7">
-        <v>0.02053049392998219</v>
+        <v>0.001297194859944284</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -892,31 +892,31 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>518</v>
+        <v>684</v>
       </c>
       <c r="D8">
-        <v>0.0006273738108575344</v>
+        <v>0.001199833932332695</v>
       </c>
       <c r="E8">
-        <v>0.2022015820257366</v>
+        <v>0.3780388489831239</v>
       </c>
       <c r="F8">
-        <v>518</v>
+        <v>684</v>
       </c>
       <c r="G8">
-        <v>0.01577108656056225</v>
+        <v>0.02844088862184435</v>
       </c>
       <c r="H8">
-        <v>0.1308854530798271</v>
+        <v>0.245931152603589</v>
       </c>
       <c r="I8">
-        <v>0.006195415859110653</v>
+        <v>0.01004169916268438</v>
       </c>
       <c r="J8">
-        <v>0.02601894538383931</v>
+        <v>0.05189107090700418</v>
       </c>
       <c r="K8">
-        <v>0.005786096910014749</v>
+        <v>0.01022336073219776</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -925,31 +925,31 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>518</v>
+        <v>59</v>
       </c>
       <c r="D9">
-        <v>0.01210114860441536</v>
+        <v>0.00385952671058476</v>
       </c>
       <c r="E9">
-        <v>0.2791609010891989</v>
+        <v>0.05054009100422263</v>
       </c>
       <c r="F9">
-        <v>518</v>
+        <v>59</v>
       </c>
       <c r="G9">
-        <v>0.02025187818799168</v>
+        <v>0.003202077932655811</v>
       </c>
       <c r="H9">
-        <v>0.1845295174280182</v>
+        <v>0.03270551166497171</v>
       </c>
       <c r="I9">
-        <v>0.009838219033554196</v>
+        <v>0.001332056242972612</v>
       </c>
       <c r="J9">
-        <v>0.03408847749233246</v>
+        <v>0.008711365284398198</v>
       </c>
       <c r="K9">
-        <v>0.007446028175763786</v>
+        <v>0.00121563533321023</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -958,31 +958,31 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>518</v>
+        <v>684</v>
       </c>
       <c r="D10">
-        <v>0.0009174455190077424</v>
+        <v>0.001812252099625766</v>
       </c>
       <c r="E10">
-        <v>0.2039270030800253</v>
+        <v>0.4078752159839496</v>
       </c>
       <c r="F10">
-        <v>518</v>
+        <v>684</v>
       </c>
       <c r="G10">
-        <v>0.01543852221220732</v>
+        <v>0.03220666048582643</v>
       </c>
       <c r="H10">
-        <v>0.1317497495329008</v>
+        <v>0.2666687830351293</v>
       </c>
       <c r="I10">
-        <v>0.007365834666416049</v>
+        <v>0.0129236081847921</v>
       </c>
       <c r="J10">
-        <v>0.02613346138969064</v>
+        <v>0.04882711649406701</v>
       </c>
       <c r="K10">
-        <v>0.005712611950002611</v>
+        <v>0.01174747699405998</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -994,7 +994,7 @@
         <v>4805</v>
       </c>
       <c r="E11">
-        <v>0.883647444890812</v>
+        <v>0.8592982107074931</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1005,31 +1005,31 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1823</v>
+        <v>85</v>
       </c>
       <c r="D12">
-        <v>0.03061900229658931</v>
+        <v>0.002475501387380064</v>
       </c>
       <c r="E12">
-        <v>0.8513227259973064</v>
+        <v>0.04337085306178778</v>
       </c>
       <c r="F12">
-        <v>1823</v>
+        <v>85</v>
       </c>
       <c r="G12">
-        <v>0.06384283024817705</v>
+        <v>0.002991055836901069</v>
       </c>
       <c r="H12">
-        <v>0.5600891294889152</v>
+        <v>0.02836394682526588</v>
       </c>
       <c r="I12">
-        <v>0.03298931068275124</v>
+        <v>0.0009896616684272885</v>
       </c>
       <c r="J12">
-        <v>0.09828316757921129</v>
+        <v>0.006671224138699472</v>
       </c>
       <c r="K12">
-        <v>0.02422631497029215</v>
+        <v>0.001111330115236342</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1038,31 +1038,31 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>730</v>
+        <v>617</v>
       </c>
       <c r="D13">
-        <v>0.0007934162858873606</v>
+        <v>0.0008665162604302168</v>
       </c>
       <c r="E13">
-        <v>0.2836754629388452</v>
+        <v>0.2870514150708914</v>
       </c>
       <c r="F13">
-        <v>730</v>
+        <v>617</v>
       </c>
       <c r="G13">
-        <v>0.0223809196613729</v>
+        <v>0.02220991323702037</v>
       </c>
       <c r="H13">
-        <v>0.1851774787064642</v>
+        <v>0.1892062119441107</v>
       </c>
       <c r="I13">
-        <v>0.007017820025794208</v>
+        <v>0.007630242151208222</v>
       </c>
       <c r="J13">
-        <v>0.03524050302803516</v>
+        <v>0.03455374017357826</v>
       </c>
       <c r="K13">
-        <v>0.008320488268509507</v>
+        <v>0.008201737073250115</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1071,31 +1071,31 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>730</v>
+        <v>85</v>
       </c>
       <c r="D14">
-        <v>0.01028321927879006</v>
+        <v>0.002971776877529919</v>
       </c>
       <c r="E14">
-        <v>0.3006821880117059</v>
+        <v>0.04787431401200593</v>
       </c>
       <c r="F14">
-        <v>730</v>
+        <v>85</v>
       </c>
       <c r="G14">
-        <v>0.02312570333015174</v>
+        <v>0.003168480703607202</v>
       </c>
       <c r="H14">
-        <v>0.1983913854928687</v>
+        <v>0.03155661758501083</v>
       </c>
       <c r="I14">
-        <v>0.008141801808960736</v>
+        <v>0.001137028448283672</v>
       </c>
       <c r="J14">
-        <v>0.03662345535121858</v>
+        <v>0.007419725530780852</v>
       </c>
       <c r="K14">
-        <v>0.008495513233356178</v>
+        <v>0.001158107188530266</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1104,31 +1104,31 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>730</v>
+        <v>617</v>
       </c>
       <c r="D15">
-        <v>0.001296792179346085</v>
+        <v>0.001197399804368615</v>
       </c>
       <c r="E15">
-        <v>0.3124301059870049</v>
+        <v>0.2643401949899271</v>
       </c>
       <c r="F15">
-        <v>730</v>
+        <v>617</v>
       </c>
       <c r="G15">
-        <v>0.02493431628681719</v>
+        <v>0.02032285393215716</v>
       </c>
       <c r="H15">
-        <v>0.2024387046694756</v>
+        <v>0.1737123600905761</v>
       </c>
       <c r="I15">
-        <v>0.009120996575802565</v>
+        <v>0.00831927452236414</v>
       </c>
       <c r="J15">
-        <v>0.03920478466898203</v>
+        <v>0.03230136178899556</v>
       </c>
       <c r="K15">
-        <v>0.009039454045705497</v>
+        <v>0.007420989568345249</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1140,7 +1140,7 @@
         <v>4805</v>
       </c>
       <c r="E16">
-        <v>1.009621520992368</v>
+        <v>1.176353588118218</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1151,31 +1151,31 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1245</v>
+        <v>97</v>
       </c>
       <c r="D17">
-        <v>0.01865265902597457</v>
+        <v>0.002722627250477672</v>
       </c>
       <c r="E17">
-        <v>0.5483171029482037</v>
+        <v>0.04655965196434408</v>
       </c>
       <c r="F17">
-        <v>1245</v>
+        <v>97</v>
       </c>
       <c r="G17">
-        <v>0.04096021328587085</v>
+        <v>0.00305652036331594</v>
       </c>
       <c r="H17">
-        <v>0.3597754908259958</v>
+        <v>0.03000462322961539</v>
       </c>
       <c r="I17">
-        <v>0.02196197852026671</v>
+        <v>0.001027111429721117</v>
       </c>
       <c r="J17">
-        <v>0.06441310828085989</v>
+        <v>0.007854246068745852</v>
       </c>
       <c r="K17">
-        <v>0.01543511194176972</v>
+        <v>0.001157607650384307</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1184,31 +1184,31 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>455</v>
+        <v>691</v>
       </c>
       <c r="D18">
-        <v>0.0005149961216375232</v>
+        <v>0.0008000775706022978</v>
       </c>
       <c r="E18">
-        <v>0.1739185689948499</v>
+        <v>0.2823822669452056</v>
       </c>
       <c r="F18">
-        <v>455</v>
+        <v>691</v>
       </c>
       <c r="G18">
-        <v>0.01389433315489441</v>
+        <v>0.02191348955966532</v>
       </c>
       <c r="H18">
-        <v>0.1133973768446594</v>
+        <v>0.1842833496630192</v>
       </c>
       <c r="I18">
-        <v>0.004485916229896247</v>
+        <v>0.008032356854528189</v>
       </c>
       <c r="J18">
-        <v>0.02178795787040144</v>
+        <v>0.03575757960788906</v>
       </c>
       <c r="K18">
-        <v>0.005020585376769304</v>
+        <v>0.00800105242524296</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1217,31 +1217,31 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>455</v>
+        <v>97</v>
       </c>
       <c r="D19">
-        <v>0.008697166456840932</v>
+        <v>0.003338298061862588</v>
       </c>
       <c r="E19">
-        <v>0.2488408359931782</v>
+        <v>0.06098816101439297</v>
       </c>
       <c r="F19">
-        <v>455</v>
+        <v>97</v>
       </c>
       <c r="G19">
-        <v>0.0189931420609355</v>
+        <v>0.003850886365398765</v>
       </c>
       <c r="H19">
-        <v>0.1638728112448007</v>
+        <v>0.03933807380963117</v>
       </c>
       <c r="I19">
-        <v>0.006947503890842199</v>
+        <v>0.001321790041401982</v>
       </c>
       <c r="J19">
-        <v>0.03112816507928073</v>
+        <v>0.01039966521784663</v>
       </c>
       <c r="K19">
-        <v>0.006911113508976996</v>
+        <v>0.00158635200932622</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1250,31 +1250,31 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>455</v>
+        <v>691</v>
       </c>
       <c r="D20">
-        <v>0.0007867485983297229</v>
+        <v>0.001357300905510783</v>
       </c>
       <c r="E20">
-        <v>0.1742072280030698</v>
+        <v>0.2997041610069573</v>
       </c>
       <c r="F20">
-        <v>455</v>
+        <v>691</v>
       </c>
       <c r="G20">
-        <v>0.01360937999561429</v>
+        <v>0.02359679853543639</v>
       </c>
       <c r="H20">
-        <v>0.1127434713998809</v>
+        <v>0.1951985992491245</v>
       </c>
       <c r="I20">
-        <v>0.005213191383518279</v>
+        <v>0.009640221367590129</v>
       </c>
       <c r="J20">
-        <v>0.02255417127162218</v>
+        <v>0.03715040034148842</v>
       </c>
       <c r="K20">
-        <v>0.004959819838404655</v>
+        <v>0.008432312519289553</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1286,7 +1286,7 @@
         <v>4805</v>
       </c>
       <c r="E21">
-        <v>0.9897040039068088</v>
+        <v>1.37943260197062</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1297,31 +1297,31 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>2169</v>
+        <v>80</v>
       </c>
       <c r="D22">
-        <v>0.03284667024854571</v>
+        <v>0.002464421442709863</v>
       </c>
       <c r="E22">
-        <v>0.8966879429062828</v>
+        <v>0.03949186997488141</v>
       </c>
       <c r="F22">
-        <v>2169</v>
+        <v>80</v>
       </c>
       <c r="G22">
-        <v>0.06800082640256733</v>
+        <v>0.002676427946425974</v>
       </c>
       <c r="H22">
-        <v>0.5866953654913232</v>
+        <v>0.0256324663059786</v>
       </c>
       <c r="I22">
-        <v>0.03994058596435934</v>
+        <v>0.0009342546109110117</v>
       </c>
       <c r="J22">
-        <v>0.1019669460365549</v>
+        <v>0.006440620636567473</v>
       </c>
       <c r="K22">
-        <v>0.02500429155770689</v>
+        <v>0.0009781229309737682</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1330,31 +1330,31 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>844</v>
+        <v>645</v>
       </c>
       <c r="D23">
-        <v>0.000826406991109252</v>
+        <v>0.0008245084900408983</v>
       </c>
       <c r="E23">
-        <v>0.2956173539860174</v>
+        <v>0.2754489569924772</v>
       </c>
       <c r="F23">
-        <v>844</v>
+        <v>645</v>
       </c>
       <c r="G23">
-        <v>0.02358393406029791</v>
+        <v>0.02135876473039389</v>
       </c>
       <c r="H23">
-        <v>0.1913351627299562</v>
+        <v>0.1799972007283941</v>
       </c>
       <c r="I23">
-        <v>0.007521819206885993</v>
+        <v>0.008024295908398926</v>
       </c>
       <c r="J23">
-        <v>0.03799583250656724</v>
+        <v>0.0347382293548435</v>
       </c>
       <c r="K23">
-        <v>0.008596397819928825</v>
+        <v>0.007764300680719316</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1363,31 +1363,31 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>844</v>
+        <v>80</v>
       </c>
       <c r="D24">
-        <v>0.01128954836167395</v>
+        <v>0.002544151502661407</v>
       </c>
       <c r="E24">
-        <v>0.3228164649335667</v>
+        <v>0.03929092094767839</v>
       </c>
       <c r="F24">
-        <v>844</v>
+        <v>80</v>
       </c>
       <c r="G24">
-        <v>0.02452081348747015</v>
+        <v>0.002686112653464079</v>
       </c>
       <c r="H24">
-        <v>0.2126501726452261</v>
+        <v>0.02556078461930156</v>
       </c>
       <c r="I24">
-        <v>0.009120725793763995</v>
+        <v>0.0009594347793608904</v>
       </c>
       <c r="J24">
-        <v>0.03968897426966578</v>
+        <v>0.006331092794425786</v>
       </c>
       <c r="K24">
-        <v>0.009195050457492471</v>
+        <v>0.000925549422390759</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1396,31 +1396,31 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>844</v>
+        <v>645</v>
       </c>
       <c r="D25">
-        <v>0.001329442718997598</v>
+        <v>0.001189700677059591</v>
       </c>
       <c r="E25">
-        <v>0.3160389759577811</v>
+        <v>0.2784969829954207</v>
       </c>
       <c r="F25">
-        <v>844</v>
+        <v>645</v>
       </c>
       <c r="G25">
-        <v>0.02509266068227589</v>
+        <v>0.02145504322834313</v>
       </c>
       <c r="H25">
-        <v>0.2045535693177953</v>
+        <v>0.1806719757150859</v>
       </c>
       <c r="I25">
-        <v>0.009361646138131618</v>
+        <v>0.009620036697015166</v>
       </c>
       <c r="J25">
-        <v>0.0400876043131575</v>
+        <v>0.03499171510338783</v>
       </c>
       <c r="K25">
-        <v>0.009019757620990276</v>
+        <v>0.007946688449010253</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1432,7 +1432,7 @@
         <v>4805</v>
       </c>
       <c r="E26">
-        <v>0.870586880017072</v>
+        <v>1.507189766038209</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1443,31 +1443,31 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1728</v>
+        <v>84.8</v>
       </c>
       <c r="D27">
-        <v>0.02818129360675812</v>
+        <v>0.003880233503878117</v>
       </c>
       <c r="E27">
-        <v>0.7776300153462217</v>
+        <v>0.06112966320943088</v>
       </c>
       <c r="F27">
-        <v>1728</v>
+        <v>84.8</v>
       </c>
       <c r="G27">
-        <v>0.05824210569262504</v>
+        <v>0.003713032533414662</v>
       </c>
       <c r="H27">
-        <v>0.5103661136003211</v>
+        <v>0.04078447029460221</v>
       </c>
       <c r="I27">
-        <v>0.03311610657256096</v>
+        <v>0.00194466314278543</v>
       </c>
       <c r="J27">
-        <v>0.08940756397787482</v>
+        <v>0.009445805405266582</v>
       </c>
       <c r="K27">
-        <v>0.0217334067914635</v>
+        <v>0.001328198099508882</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1476,31 +1476,31 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>652.4</v>
+        <v>695.6</v>
       </c>
       <c r="D28">
-        <v>0.000706125283613801</v>
+        <v>0.001009197626262903</v>
       </c>
       <c r="E28">
-        <v>0.2449661223916337</v>
+        <v>0.3337541255867109</v>
       </c>
       <c r="F28">
-        <v>652.4</v>
+        <v>695.6</v>
       </c>
       <c r="G28">
-        <v>0.01934965865220874</v>
+        <v>0.02567309096921235</v>
       </c>
       <c r="H28">
-        <v>0.1593924776650965</v>
+        <v>0.2174323295475915</v>
       </c>
       <c r="I28">
-        <v>0.006384886219166219</v>
+        <v>0.009983355016447603</v>
       </c>
       <c r="J28">
-        <v>0.03100065493490547</v>
+        <v>0.04282717441674322</v>
       </c>
       <c r="K28">
-        <v>0.007097708596847952</v>
+        <v>0.009326099511235952</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1509,31 +1509,31 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>652.4</v>
+        <v>84.8</v>
       </c>
       <c r="D29">
-        <v>0.01121693800669163</v>
+        <v>0.003681824984960258</v>
       </c>
       <c r="E29">
-        <v>0.2999003092059865</v>
+        <v>0.05978160239756107</v>
       </c>
       <c r="F29">
-        <v>652.4</v>
+        <v>84.8</v>
       </c>
       <c r="G29">
-        <v>0.02266765860840678</v>
+        <v>0.005260115978308022</v>
       </c>
       <c r="H29">
-        <v>0.1977146023651585</v>
+        <v>0.03815147946588695</v>
       </c>
       <c r="I29">
-        <v>0.008761357585899531</v>
+        <v>0.001344716642051935</v>
       </c>
       <c r="J29">
-        <v>0.03705475144088268</v>
+        <v>0.00940621888730675</v>
       </c>
       <c r="K29">
-        <v>0.008321506949141622</v>
+        <v>0.001411487767472863</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1542,31 +1542,31 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>652.4</v>
+        <v>695.6</v>
       </c>
       <c r="D30">
-        <v>0.001126003381796181</v>
+        <v>0.001507416204549372</v>
       </c>
       <c r="E30">
-        <v>0.2635461474070325</v>
+        <v>0.3400745362043381</v>
       </c>
       <c r="F30">
-        <v>652.4</v>
+        <v>695.6</v>
       </c>
       <c r="G30">
-        <v>0.02073489734902978</v>
+        <v>0.02668694527819753</v>
       </c>
       <c r="H30">
-        <v>0.1707280148519203</v>
+        <v>0.2217794653959572</v>
       </c>
       <c r="I30">
-        <v>0.008045240817591549</v>
+        <v>0.01103544312063605</v>
       </c>
       <c r="J30">
-        <v>0.03331172454636544</v>
+        <v>0.0415131954010576</v>
       </c>
       <c r="K30">
-        <v>0.007555293967016041</v>
+        <v>0.009725327230989933</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1578,7 +1578,7 @@
         <v>4805</v>
       </c>
       <c r="E31">
-        <v>0.9661777171539143</v>
+        <v>1.19691661009565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new class `ChangeKeysDict` which subclasses collections.UserDict. The purpose is for allowing keys to change during a dict's lifetime, and ensure all references to changed key will also be updated
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -716,28 +716,28 @@
         <v>103</v>
       </c>
       <c r="D2">
-        <v>0.008189005544409156</v>
+        <v>0.007322581950575113</v>
       </c>
       <c r="E2">
-        <v>0.105924578034319</v>
+        <v>0.1018237750977278</v>
       </c>
       <c r="F2">
         <v>103</v>
       </c>
       <c r="G2">
-        <v>0.005882885656319559</v>
+        <v>0.007695870008319616</v>
       </c>
       <c r="H2">
-        <v>0.06969061761628836</v>
+        <v>0.06681700050830841</v>
       </c>
       <c r="I2">
-        <v>0.005414729355834424</v>
+        <v>0.002055973745882511</v>
       </c>
       <c r="J2">
-        <v>0.01658011670224369</v>
+        <v>0.01516876369714737</v>
       </c>
       <c r="K2">
-        <v>0.002096734941005707</v>
+        <v>0.002399732824414968</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -749,28 +749,28 @@
         <v>841</v>
       </c>
       <c r="D3">
-        <v>0.001355051877908409</v>
+        <v>0.001035409513860941</v>
       </c>
       <c r="E3">
-        <v>0.4458491399418563</v>
+        <v>0.3582811197265983</v>
       </c>
       <c r="F3">
         <v>841</v>
       </c>
       <c r="G3">
-        <v>0.03444239869713783</v>
+        <v>0.02867878833785653</v>
       </c>
       <c r="H3">
-        <v>0.2877437327988446</v>
+        <v>0.2299934513866901</v>
       </c>
       <c r="I3">
-        <v>0.0161881810054183</v>
+        <v>0.01015108777210116</v>
       </c>
       <c r="J3">
-        <v>0.0571952520404011</v>
+        <v>0.04752691462635994</v>
       </c>
       <c r="K3">
-        <v>0.01244004664476961</v>
+        <v>0.01020820811390877</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -782,28 +782,28 @@
         <v>103</v>
       </c>
       <c r="D4">
-        <v>0.005695371772162616</v>
+        <v>0.008836568333208561</v>
       </c>
       <c r="E4">
-        <v>0.1002145250095055</v>
+        <v>0.1292784819379449</v>
       </c>
       <c r="F4">
         <v>103</v>
       </c>
       <c r="G4">
-        <v>0.01339302223641425</v>
+        <v>0.009095696732401848</v>
       </c>
       <c r="H4">
-        <v>0.06159640965051949</v>
+        <v>0.08478125417605042</v>
       </c>
       <c r="I4">
-        <v>0.001973273698240519</v>
+        <v>0.002608806826174259</v>
       </c>
       <c r="J4">
-        <v>0.01416924560908228</v>
+        <v>0.01961160218343139</v>
       </c>
       <c r="K4">
-        <v>0.002171794883906841</v>
+        <v>0.003228395711630583</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -815,28 +815,28 @@
         <v>841</v>
       </c>
       <c r="D5">
-        <v>0.001980427536182106</v>
+        <v>0.001646819058805704</v>
       </c>
       <c r="E5">
-        <v>0.4499561260454357</v>
+        <v>0.4029014273546636</v>
       </c>
       <c r="F5">
         <v>841</v>
       </c>
       <c r="G5">
-        <v>0.03585337020922452</v>
+        <v>0.03182772826403379</v>
       </c>
       <c r="H5">
-        <v>0.2926456088898703</v>
+        <v>0.2593141803517938</v>
       </c>
       <c r="I5">
-        <v>0.01467407483141869</v>
+        <v>0.01358586363494396</v>
       </c>
       <c r="J5">
-        <v>0.05429538327734917</v>
+        <v>0.05136972526088357</v>
       </c>
       <c r="K5">
-        <v>0.01307916862424463</v>
+        <v>0.01172052184119821</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -848,7 +848,7 @@
         <v>4805</v>
       </c>
       <c r="E6">
-        <v>1.062308883643709</v>
+        <v>0.9538764897733927</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -862,28 +862,28 @@
         <v>59</v>
       </c>
       <c r="D7">
-        <v>0.003549611894413829</v>
+        <v>0.005482353270053864</v>
       </c>
       <c r="E7">
-        <v>0.0703013630118221</v>
+        <v>0.07444539573043585</v>
       </c>
       <c r="F7">
         <v>59</v>
       </c>
       <c r="G7">
-        <v>0.003958272864110768</v>
+        <v>0.004859731066972017</v>
       </c>
       <c r="H7">
-        <v>0.05023069749586284</v>
+        <v>0.04732069931924343</v>
       </c>
       <c r="I7">
-        <v>0.001357558649033308</v>
+        <v>0.001852010376751423</v>
       </c>
       <c r="J7">
-        <v>0.009682819480076432</v>
+        <v>0.01368260616436601</v>
       </c>
       <c r="K7">
-        <v>0.001297194859944284</v>
+        <v>0.001672299578785896</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -895,28 +895,28 @@
         <v>684</v>
       </c>
       <c r="D8">
-        <v>0.001199833932332695</v>
+        <v>0.0008758548647165298</v>
       </c>
       <c r="E8">
-        <v>0.3780388489831239</v>
+        <v>0.2877091160044074</v>
       </c>
       <c r="F8">
         <v>684</v>
       </c>
       <c r="G8">
-        <v>0.02844088862184435</v>
+        <v>0.02327139861881733</v>
       </c>
       <c r="H8">
-        <v>0.245931152603589</v>
+        <v>0.1859019221737981</v>
       </c>
       <c r="I8">
-        <v>0.01004169916268438</v>
+        <v>0.007711600512266159</v>
       </c>
       <c r="J8">
-        <v>0.05189107090700418</v>
+        <v>0.0370238465256989</v>
       </c>
       <c r="K8">
-        <v>0.01022336073219776</v>
+        <v>0.00832445127889514</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -928,28 +928,28 @@
         <v>59</v>
       </c>
       <c r="D9">
-        <v>0.00385952671058476</v>
+        <v>0.006412862800061703</v>
       </c>
       <c r="E9">
-        <v>0.05054009100422263</v>
+        <v>0.09168151998892426</v>
       </c>
       <c r="F9">
         <v>59</v>
       </c>
       <c r="G9">
-        <v>0.003202077932655811</v>
+        <v>0.006185937207192183</v>
       </c>
       <c r="H9">
-        <v>0.03270551166497171</v>
+        <v>0.05912051210179925</v>
       </c>
       <c r="I9">
-        <v>0.001332056242972612</v>
+        <v>0.002011967822909355</v>
       </c>
       <c r="J9">
-        <v>0.008711365284398198</v>
+        <v>0.01534664677456021</v>
       </c>
       <c r="K9">
-        <v>0.00121563533321023</v>
+        <v>0.002233991865068674</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -961,28 +961,28 @@
         <v>684</v>
       </c>
       <c r="D10">
-        <v>0.001812252099625766</v>
+        <v>0.001465102192014456</v>
       </c>
       <c r="E10">
-        <v>0.4078752159839496</v>
+        <v>0.3535058093257248</v>
       </c>
       <c r="F10">
         <v>684</v>
       </c>
       <c r="G10">
-        <v>0.03220666048582643</v>
+        <v>0.02789804013445973</v>
       </c>
       <c r="H10">
-        <v>0.2666687830351293</v>
+        <v>0.2279132469557226</v>
       </c>
       <c r="I10">
-        <v>0.0129236081847921</v>
+        <v>0.01136909332126379</v>
       </c>
       <c r="J10">
-        <v>0.04882711649406701</v>
+        <v>0.04438761109486222</v>
       </c>
       <c r="K10">
-        <v>0.01174747699405998</v>
+        <v>0.01026897225528955</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -994,7 +994,7 @@
         <v>4805</v>
       </c>
       <c r="E11">
-        <v>0.8592982107074931</v>
+        <v>0.8631404815241694</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1008,28 +1008,28 @@
         <v>85</v>
       </c>
       <c r="D12">
-        <v>0.002475501387380064</v>
+        <v>0.003124778624624014</v>
       </c>
       <c r="E12">
-        <v>0.04337085306178778</v>
+        <v>0.05461055412888527</v>
       </c>
       <c r="F12">
         <v>85</v>
       </c>
       <c r="G12">
-        <v>0.002991055836901069</v>
+        <v>0.003828324377536774</v>
       </c>
       <c r="H12">
-        <v>0.02836394682526588</v>
+        <v>0.0354169849306345</v>
       </c>
       <c r="I12">
-        <v>0.0009896616684272885</v>
+        <v>0.001112679019570351</v>
       </c>
       <c r="J12">
-        <v>0.006671224138699472</v>
+        <v>0.00840382743626833</v>
       </c>
       <c r="K12">
-        <v>0.001111330115236342</v>
+        <v>0.001416357234120369</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1041,28 +1041,28 @@
         <v>617</v>
       </c>
       <c r="D13">
-        <v>0.0008665162604302168</v>
+        <v>0.000872946809977293</v>
       </c>
       <c r="E13">
-        <v>0.2870514150708914</v>
+        <v>0.2777701411396265</v>
       </c>
       <c r="F13">
         <v>617</v>
       </c>
       <c r="G13">
-        <v>0.02220991323702037</v>
+        <v>0.02208305709064007</v>
       </c>
       <c r="H13">
-        <v>0.1892062119441107</v>
+        <v>0.1790438904426992</v>
       </c>
       <c r="I13">
-        <v>0.007630242151208222</v>
+        <v>0.007510946597903967</v>
       </c>
       <c r="J13">
-        <v>0.03455374017357826</v>
+        <v>0.0364212105050683</v>
       </c>
       <c r="K13">
-        <v>0.008201737073250115</v>
+        <v>0.008111270610243082</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1074,28 +1074,28 @@
         <v>85</v>
       </c>
       <c r="D14">
-        <v>0.002971776877529919</v>
+        <v>0.002861146815121174</v>
       </c>
       <c r="E14">
-        <v>0.04787431401200593</v>
+        <v>0.04968480579555035</v>
       </c>
       <c r="F14">
         <v>85</v>
       </c>
       <c r="G14">
-        <v>0.003168480703607202</v>
+        <v>0.003280565142631531</v>
       </c>
       <c r="H14">
-        <v>0.03155661758501083</v>
+        <v>0.03195054223760962</v>
       </c>
       <c r="I14">
-        <v>0.001137028448283672</v>
+        <v>0.001105108764022589</v>
       </c>
       <c r="J14">
-        <v>0.007419725530780852</v>
+        <v>0.008586075156927109</v>
       </c>
       <c r="K14">
-        <v>0.001158107188530266</v>
+        <v>0.001208995468914509</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1107,28 +1107,28 @@
         <v>617</v>
       </c>
       <c r="D15">
-        <v>0.001197399804368615</v>
+        <v>0.001343375537544489</v>
       </c>
       <c r="E15">
-        <v>0.2643401949899271</v>
+        <v>0.2845779629424214</v>
       </c>
       <c r="F15">
         <v>617</v>
       </c>
       <c r="G15">
-        <v>0.02032285393215716</v>
+        <v>0.02225219598039985</v>
       </c>
       <c r="H15">
-        <v>0.1737123600905761</v>
+        <v>0.1848116684705019</v>
       </c>
       <c r="I15">
-        <v>0.00831927452236414</v>
+        <v>0.009134972468018532</v>
       </c>
       <c r="J15">
-        <v>0.03230136178899556</v>
+        <v>0.03530557407066226</v>
       </c>
       <c r="K15">
-        <v>0.007420989568345249</v>
+        <v>0.00816273083910346</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1140,7 +1140,7 @@
         <v>4805</v>
       </c>
       <c r="E16">
-        <v>1.176353588118218</v>
+        <v>0.9390419572591782</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1154,28 +1154,28 @@
         <v>97</v>
       </c>
       <c r="D17">
-        <v>0.002722627250477672</v>
+        <v>0.003192984033375978</v>
       </c>
       <c r="E17">
-        <v>0.04655965196434408</v>
+        <v>0.05968657089397311</v>
       </c>
       <c r="F17">
         <v>97</v>
       </c>
       <c r="G17">
-        <v>0.00305652036331594</v>
+        <v>0.004223072435706854</v>
       </c>
       <c r="H17">
-        <v>0.03000462322961539</v>
+        <v>0.03784104296937585</v>
       </c>
       <c r="I17">
-        <v>0.001027111429721117</v>
+        <v>0.001122236251831055</v>
       </c>
       <c r="J17">
-        <v>0.007854246068745852</v>
+        <v>0.01052592322230339</v>
       </c>
       <c r="K17">
-        <v>0.001157607650384307</v>
+        <v>0.001527272164821625</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1187,28 +1187,28 @@
         <v>691</v>
       </c>
       <c r="D18">
-        <v>0.0008000775706022978</v>
+        <v>0.0009333062916994095</v>
       </c>
       <c r="E18">
-        <v>0.2823822669452056</v>
+        <v>0.3100540842860937</v>
       </c>
       <c r="F18">
         <v>691</v>
       </c>
       <c r="G18">
-        <v>0.02191348955966532</v>
+        <v>0.02490810491144657</v>
       </c>
       <c r="H18">
-        <v>0.1842833496630192</v>
+        <v>0.2005890929140151</v>
       </c>
       <c r="I18">
-        <v>0.008032356854528189</v>
+        <v>0.0086867930367589</v>
       </c>
       <c r="J18">
-        <v>0.03575757960788906</v>
+        <v>0.03949838085100055</v>
       </c>
       <c r="K18">
-        <v>0.00800105242524296</v>
+        <v>0.008871165569871664</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1220,28 +1220,28 @@
         <v>97</v>
       </c>
       <c r="D19">
-        <v>0.003338298061862588</v>
+        <v>0.002967767417430878</v>
       </c>
       <c r="E19">
-        <v>0.06098816101439297</v>
+        <v>0.051557338796556</v>
       </c>
       <c r="F19">
         <v>97</v>
       </c>
       <c r="G19">
-        <v>0.003850886365398765</v>
+        <v>0.003638145979493856</v>
       </c>
       <c r="H19">
-        <v>0.03933807380963117</v>
+        <v>0.03314039576798677</v>
       </c>
       <c r="I19">
-        <v>0.001321790041401982</v>
+        <v>0.00109127489849925</v>
       </c>
       <c r="J19">
-        <v>0.01039966521784663</v>
+        <v>0.008736977819353342</v>
       </c>
       <c r="K19">
-        <v>0.00158635200932622</v>
+        <v>0.001243905164301395</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1253,28 +1253,28 @@
         <v>691</v>
       </c>
       <c r="D20">
-        <v>0.001357300905510783</v>
+        <v>0.001468064729124308</v>
       </c>
       <c r="E20">
-        <v>0.2997041610069573</v>
+        <v>0.3119523008354008</v>
       </c>
       <c r="F20">
         <v>691</v>
       </c>
       <c r="G20">
-        <v>0.02359679853543639</v>
+        <v>0.02475325390696526</v>
       </c>
       <c r="H20">
-        <v>0.1951985992491245</v>
+        <v>0.2021430507302284</v>
       </c>
       <c r="I20">
-        <v>0.009640221367590129</v>
+        <v>0.009953280445188284</v>
       </c>
       <c r="J20">
-        <v>0.03715040034148842</v>
+        <v>0.03843353502452374</v>
       </c>
       <c r="K20">
-        <v>0.008432312519289553</v>
+        <v>0.008988030254840851</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1286,7 +1286,7 @@
         <v>4805</v>
       </c>
       <c r="E21">
-        <v>1.37943260197062</v>
+        <v>0.9581344211474061</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1300,28 +1300,28 @@
         <v>80</v>
       </c>
       <c r="D22">
-        <v>0.002464421442709863</v>
+        <v>0.002981758210808039</v>
       </c>
       <c r="E22">
-        <v>0.03949186997488141</v>
+        <v>0.05135160824283957</v>
       </c>
       <c r="F22">
         <v>80</v>
       </c>
       <c r="G22">
-        <v>0.002676427946425974</v>
+        <v>0.003661919850856066</v>
       </c>
       <c r="H22">
-        <v>0.0256324663059786</v>
+        <v>0.03342994069680572</v>
       </c>
       <c r="I22">
-        <v>0.0009342546109110117</v>
+        <v>0.001056331675499678</v>
       </c>
       <c r="J22">
-        <v>0.006440620636567473</v>
+        <v>0.007929214742034674</v>
       </c>
       <c r="K22">
-        <v>0.0009781229309737682</v>
+        <v>0.001306978985667229</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1333,28 +1333,28 @@
         <v>645</v>
       </c>
       <c r="D23">
-        <v>0.0008245084900408983</v>
+        <v>0.0008408799767494202</v>
       </c>
       <c r="E23">
-        <v>0.2754489569924772</v>
+        <v>0.2793110520578921</v>
       </c>
       <c r="F23">
         <v>645</v>
       </c>
       <c r="G23">
-        <v>0.02135876473039389</v>
+        <v>0.02277254359796643</v>
       </c>
       <c r="H23">
-        <v>0.1799972007283941</v>
+        <v>0.1806641155853868</v>
       </c>
       <c r="I23">
-        <v>0.008024295908398926</v>
+        <v>0.007609287276864052</v>
       </c>
       <c r="J23">
-        <v>0.0347382293548435</v>
+        <v>0.0350108789280057</v>
       </c>
       <c r="K23">
-        <v>0.007764300680719316</v>
+        <v>0.008100660517811775</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1366,28 +1366,28 @@
         <v>80</v>
       </c>
       <c r="D24">
-        <v>0.002544151502661407</v>
+        <v>0.002797433640807867</v>
       </c>
       <c r="E24">
-        <v>0.03929092094767839</v>
+        <v>0.04392475681379437</v>
       </c>
       <c r="F24">
         <v>80</v>
       </c>
       <c r="G24">
-        <v>0.002686112653464079</v>
+        <v>0.003027439117431641</v>
       </c>
       <c r="H24">
-        <v>0.02556078461930156</v>
+        <v>0.02779966033995152</v>
       </c>
       <c r="I24">
-        <v>0.0009594347793608904</v>
+        <v>0.0009687785059213638</v>
       </c>
       <c r="J24">
-        <v>0.006331092794425786</v>
+        <v>0.007670196704566479</v>
       </c>
       <c r="K24">
-        <v>0.000925549422390759</v>
+        <v>0.001151410862803459</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1399,28 +1399,28 @@
         <v>645</v>
       </c>
       <c r="D25">
-        <v>0.001189700677059591</v>
+        <v>0.001083121635019779</v>
       </c>
       <c r="E25">
-        <v>0.2784969829954207</v>
+        <v>0.2651075110770762</v>
       </c>
       <c r="F25">
         <v>645</v>
       </c>
       <c r="G25">
-        <v>0.02145504322834313</v>
+        <v>0.02058612275868654</v>
       </c>
       <c r="H25">
-        <v>0.1806719757150859</v>
+        <v>0.1708462117239833</v>
       </c>
       <c r="I25">
-        <v>0.009620036697015166</v>
+        <v>0.008810519706457853</v>
       </c>
       <c r="J25">
-        <v>0.03499171510338783</v>
+        <v>0.0340973143465817</v>
       </c>
       <c r="K25">
-        <v>0.007946688449010253</v>
+        <v>0.007779397536069155</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1432,7 +1432,7 @@
         <v>4805</v>
       </c>
       <c r="E26">
-        <v>1.507189766038209</v>
+        <v>1.1352184927091</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1446,28 +1446,28 @@
         <v>84.8</v>
       </c>
       <c r="D27">
-        <v>0.003880233503878117</v>
+        <v>0.004420891217887401</v>
       </c>
       <c r="E27">
-        <v>0.06112966320943088</v>
+        <v>0.06838358081877231</v>
       </c>
       <c r="F27">
         <v>84.8</v>
       </c>
       <c r="G27">
-        <v>0.003713032533414662</v>
+        <v>0.004853783547878266</v>
       </c>
       <c r="H27">
-        <v>0.04078447029460221</v>
+        <v>0.04416513368487358</v>
       </c>
       <c r="I27">
-        <v>0.00194466314278543</v>
+        <v>0.001439846213907003</v>
       </c>
       <c r="J27">
-        <v>0.009445805405266582</v>
+        <v>0.01114206705242395</v>
       </c>
       <c r="K27">
-        <v>0.001328198099508882</v>
+        <v>0.001664528157562017</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1479,28 +1479,28 @@
         <v>695.6</v>
       </c>
       <c r="D28">
-        <v>0.001009197626262903</v>
+        <v>0.0009116794914007187</v>
       </c>
       <c r="E28">
-        <v>0.3337541255867109</v>
+        <v>0.3026251026429236</v>
       </c>
       <c r="F28">
         <v>695.6</v>
       </c>
       <c r="G28">
-        <v>0.02567309096921235</v>
+        <v>0.02434277851134539</v>
       </c>
       <c r="H28">
-        <v>0.2174323295475915</v>
+        <v>0.1952384945005178</v>
       </c>
       <c r="I28">
-        <v>0.009983355016447603</v>
+        <v>0.008333943039178848</v>
       </c>
       <c r="J28">
-        <v>0.04282717441674322</v>
+        <v>0.03909624628722667</v>
       </c>
       <c r="K28">
-        <v>0.009326099511235952</v>
+        <v>0.008723151218146086</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1512,28 +1512,28 @@
         <v>84.8</v>
       </c>
       <c r="D29">
-        <v>0.003681824984960258</v>
+        <v>0.004775155801326036</v>
       </c>
       <c r="E29">
-        <v>0.05978160239756107</v>
+        <v>0.07322538066655397</v>
       </c>
       <c r="F29">
         <v>84.8</v>
       </c>
       <c r="G29">
-        <v>0.005260115978308022</v>
+        <v>0.005045556835830212</v>
       </c>
       <c r="H29">
-        <v>0.03815147946588695</v>
+        <v>0.04735847292467952</v>
       </c>
       <c r="I29">
-        <v>0.001344716642051935</v>
+        <v>0.001557187363505363</v>
       </c>
       <c r="J29">
-        <v>0.00940621888730675</v>
+        <v>0.01199029972776771</v>
       </c>
       <c r="K29">
-        <v>0.001411487767472863</v>
+        <v>0.001813339814543724</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1545,28 +1545,28 @@
         <v>695.6</v>
       </c>
       <c r="D30">
-        <v>0.001507416204549372</v>
+        <v>0.001401296630501747</v>
       </c>
       <c r="E30">
-        <v>0.3400745362043381</v>
+        <v>0.3236090023070574</v>
       </c>
       <c r="F30">
         <v>695.6</v>
       </c>
       <c r="G30">
-        <v>0.02668694527819753</v>
+        <v>0.02546346820890904</v>
       </c>
       <c r="H30">
-        <v>0.2217794653959572</v>
+        <v>0.209005671646446</v>
       </c>
       <c r="I30">
-        <v>0.01103544312063605</v>
+        <v>0.01057074591517448</v>
       </c>
       <c r="J30">
-        <v>0.0415131954010576</v>
+        <v>0.0407187519595027</v>
       </c>
       <c r="K30">
-        <v>0.009725327230989933</v>
+        <v>0.009383930545300245</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1578,7 +1578,7 @@
         <v>4805</v>
       </c>
       <c r="E31">
-        <v>1.19691661009565</v>
+        <v>0.9698823684826493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged framework will now check all feasible paths for a recently merged component prior to the next nomination phase. This is required because merging may bump up the merged component's gmin leading to skipping
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -716,28 +716,28 @@
         <v>103</v>
       </c>
       <c r="D2">
-        <v>0.007322581950575113</v>
+        <v>0.004212758503854275</v>
       </c>
       <c r="E2">
-        <v>0.1018237750977278</v>
+        <v>0.0673017748631537</v>
       </c>
       <c r="F2">
         <v>103</v>
       </c>
       <c r="G2">
-        <v>0.007695870008319616</v>
+        <v>0.004141566343605518</v>
       </c>
       <c r="H2">
-        <v>0.06681700050830841</v>
+        <v>0.04282997362315655</v>
       </c>
       <c r="I2">
-        <v>0.002055973745882511</v>
+        <v>0.001827794127166271</v>
       </c>
       <c r="J2">
-        <v>0.01516876369714737</v>
+        <v>0.01286618737503886</v>
       </c>
       <c r="K2">
-        <v>0.002399732824414968</v>
+        <v>0.001410416327416897</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -749,28 +749,28 @@
         <v>841</v>
       </c>
       <c r="D3">
-        <v>0.001035409513860941</v>
+        <v>0.001007826998829842</v>
       </c>
       <c r="E3">
-        <v>0.3582811197265983</v>
+        <v>0.3842693129554391</v>
       </c>
       <c r="F3">
         <v>841</v>
       </c>
       <c r="G3">
-        <v>0.02867878833785653</v>
+        <v>0.02702527865767479</v>
       </c>
       <c r="H3">
-        <v>0.2299934513866901</v>
+        <v>0.2381146480329335</v>
       </c>
       <c r="I3">
-        <v>0.01015108777210116</v>
+        <v>0.01914155157282948</v>
       </c>
       <c r="J3">
-        <v>0.04752691462635994</v>
+        <v>0.06134908180683851</v>
       </c>
       <c r="K3">
-        <v>0.01020820811390877</v>
+        <v>0.009389501065015793</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -782,28 +782,28 @@
         <v>103</v>
       </c>
       <c r="D4">
-        <v>0.008836568333208561</v>
+        <v>0.004408972337841988</v>
       </c>
       <c r="E4">
-        <v>0.1292784819379449</v>
+        <v>0.06654203357174993</v>
       </c>
       <c r="F4">
         <v>103</v>
       </c>
       <c r="G4">
-        <v>0.009095696732401848</v>
+        <v>0.004251713398844004</v>
       </c>
       <c r="H4">
-        <v>0.08478125417605042</v>
+        <v>0.04214417422190309</v>
       </c>
       <c r="I4">
-        <v>0.002608806826174259</v>
+        <v>0.001718732062727213</v>
       </c>
       <c r="J4">
-        <v>0.01961160218343139</v>
+        <v>0.01264319103211164</v>
       </c>
       <c r="K4">
-        <v>0.003228395711630583</v>
+        <v>0.001474219374358654</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -815,28 +815,28 @@
         <v>841</v>
       </c>
       <c r="D5">
-        <v>0.001646819058805704</v>
+        <v>0.001479329541325569</v>
       </c>
       <c r="E5">
-        <v>0.4029014273546636</v>
+        <v>0.383428439963609</v>
       </c>
       <c r="F5">
         <v>841</v>
       </c>
       <c r="G5">
-        <v>0.03182772826403379</v>
+        <v>0.02749304007738829</v>
       </c>
       <c r="H5">
-        <v>0.2593141803517938</v>
+        <v>0.2364881676621735</v>
       </c>
       <c r="I5">
-        <v>0.01358586363494396</v>
+        <v>0.0199749581515789</v>
       </c>
       <c r="J5">
-        <v>0.05136972526088357</v>
+        <v>0.06070742849260569</v>
       </c>
       <c r="K5">
-        <v>0.01172052184119821</v>
+        <v>0.009437066502869129</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -848,7 +848,7 @@
         <v>4805</v>
       </c>
       <c r="E6">
-        <v>0.9538764897733927</v>
+        <v>1.035875022411346</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -862,28 +862,28 @@
         <v>59</v>
       </c>
       <c r="D7">
-        <v>0.005482353270053864</v>
+        <v>0.004190638661384583</v>
       </c>
       <c r="E7">
-        <v>0.07444539573043585</v>
+        <v>0.06552575435489416</v>
       </c>
       <c r="F7">
         <v>59</v>
       </c>
       <c r="G7">
-        <v>0.004859731066972017</v>
+        <v>0.004033647943288088</v>
       </c>
       <c r="H7">
-        <v>0.04732069931924343</v>
+        <v>0.04086672281846404</v>
       </c>
       <c r="I7">
-        <v>0.001852010376751423</v>
+        <v>0.00188658619299531</v>
       </c>
       <c r="J7">
-        <v>0.01368260616436601</v>
+        <v>0.01274234103038907</v>
       </c>
       <c r="K7">
-        <v>0.001672299578785896</v>
+        <v>0.001625906210392714</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -895,28 +895,28 @@
         <v>684</v>
       </c>
       <c r="D8">
-        <v>0.0008758548647165298</v>
+        <v>0.0009196139872074127</v>
       </c>
       <c r="E8">
-        <v>0.2877091160044074</v>
+        <v>0.3518870892003179</v>
       </c>
       <c r="F8">
         <v>684</v>
       </c>
       <c r="G8">
-        <v>0.02327139861881733</v>
+        <v>0.02473711036145687</v>
       </c>
       <c r="H8">
-        <v>0.1859019221737981</v>
+        <v>0.2196963313035667</v>
       </c>
       <c r="I8">
-        <v>0.007711600512266159</v>
+        <v>0.01750291045755148</v>
       </c>
       <c r="J8">
-        <v>0.0370238465256989</v>
+        <v>0.05480776494368911</v>
       </c>
       <c r="K8">
-        <v>0.00832445127889514</v>
+        <v>0.008440659381449223</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -928,28 +928,28 @@
         <v>59</v>
       </c>
       <c r="D9">
-        <v>0.006412862800061703</v>
+        <v>0.004432704299688339</v>
       </c>
       <c r="E9">
-        <v>0.09168151998892426</v>
+        <v>0.06589768594130874</v>
       </c>
       <c r="F9">
         <v>59</v>
       </c>
       <c r="G9">
-        <v>0.006185937207192183</v>
+        <v>0.004031843040138483</v>
       </c>
       <c r="H9">
-        <v>0.05912051210179925</v>
+        <v>0.04140257462859154</v>
       </c>
       <c r="I9">
-        <v>0.002011967822909355</v>
+        <v>0.001947587821632624</v>
       </c>
       <c r="J9">
-        <v>0.01534664677456021</v>
+        <v>0.01288035791367292</v>
       </c>
       <c r="K9">
-        <v>0.002233991865068674</v>
+        <v>0.001401062123477459</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -961,28 +961,28 @@
         <v>684</v>
       </c>
       <c r="D10">
-        <v>0.001465102192014456</v>
+        <v>0.001342307776212692</v>
       </c>
       <c r="E10">
-        <v>0.3535058093257248</v>
+        <v>0.3479090337641537</v>
       </c>
       <c r="F10">
         <v>684</v>
       </c>
       <c r="G10">
-        <v>0.02789804013445973</v>
+        <v>0.02436545863747597</v>
       </c>
       <c r="H10">
-        <v>0.2279132469557226</v>
+        <v>0.2163986614905298</v>
       </c>
       <c r="I10">
-        <v>0.01136909332126379</v>
+        <v>0.01830550003796816</v>
       </c>
       <c r="J10">
-        <v>0.04438761109486222</v>
+        <v>0.05400724289938807</v>
       </c>
       <c r="K10">
-        <v>0.01026897225528955</v>
+        <v>0.008495531510561705</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -994,7 +994,7 @@
         <v>4805</v>
       </c>
       <c r="E11">
-        <v>0.8631404815241694</v>
+        <v>0.9173209187574685</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1008,28 +1008,28 @@
         <v>85</v>
       </c>
       <c r="D12">
-        <v>0.003124778624624014</v>
+        <v>0.002281279303133488</v>
       </c>
       <c r="E12">
-        <v>0.05461055412888527</v>
+        <v>0.04406110802665353</v>
       </c>
       <c r="F12">
         <v>85</v>
       </c>
       <c r="G12">
-        <v>0.003828324377536774</v>
+        <v>0.002785990480333567</v>
       </c>
       <c r="H12">
-        <v>0.0354169849306345</v>
+        <v>0.02779335854575038</v>
       </c>
       <c r="I12">
-        <v>0.001112679019570351</v>
+        <v>0.001289741136133671</v>
       </c>
       <c r="J12">
-        <v>0.00840382743626833</v>
+        <v>0.008218399249017239</v>
       </c>
       <c r="K12">
-        <v>0.001416357234120369</v>
+        <v>0.000989789143204689</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1041,28 +1041,28 @@
         <v>617</v>
       </c>
       <c r="D13">
-        <v>0.000872946809977293</v>
+        <v>0.0007802830077707767</v>
       </c>
       <c r="E13">
-        <v>0.2777701411396265</v>
+        <v>0.2830429808236659</v>
       </c>
       <c r="F13">
         <v>617</v>
       </c>
       <c r="G13">
-        <v>0.02208305709064007</v>
+        <v>0.01978500094264746</v>
       </c>
       <c r="H13">
-        <v>0.1790438904426992</v>
+        <v>0.1763087250292301</v>
       </c>
       <c r="I13">
-        <v>0.007510946597903967</v>
+        <v>0.01511721638962626</v>
       </c>
       <c r="J13">
-        <v>0.0364212105050683</v>
+        <v>0.04328344948589802</v>
       </c>
       <c r="K13">
-        <v>0.008111270610243082</v>
+        <v>0.006938849110156298</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1074,28 +1074,28 @@
         <v>85</v>
       </c>
       <c r="D14">
-        <v>0.002861146815121174</v>
+        <v>0.002703116741031408</v>
       </c>
       <c r="E14">
-        <v>0.04968480579555035</v>
+        <v>0.05076680891215801</v>
       </c>
       <c r="F14">
         <v>85</v>
       </c>
       <c r="G14">
-        <v>0.003280565142631531</v>
+        <v>0.003207582049071789</v>
       </c>
       <c r="H14">
-        <v>0.03195054223760962</v>
+        <v>0.03228841535747051</v>
       </c>
       <c r="I14">
-        <v>0.001105108764022589</v>
+        <v>0.001373117789626122</v>
       </c>
       <c r="J14">
-        <v>0.008586075156927109</v>
+        <v>0.009126319549977779</v>
       </c>
       <c r="K14">
-        <v>0.001208995468914509</v>
+        <v>0.001129476819187403</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1107,28 +1107,28 @@
         <v>617</v>
       </c>
       <c r="D15">
-        <v>0.001343375537544489</v>
+        <v>0.001154396682977676</v>
       </c>
       <c r="E15">
-        <v>0.2845779629424214</v>
+        <v>0.2906279531307518</v>
       </c>
       <c r="F15">
         <v>617</v>
       </c>
       <c r="G15">
-        <v>0.02225219598039985</v>
+        <v>0.02061355207115412</v>
       </c>
       <c r="H15">
-        <v>0.1848116684705019</v>
+        <v>0.1800362728536129</v>
       </c>
       <c r="I15">
-        <v>0.009134972468018532</v>
+        <v>0.01625634403899312</v>
       </c>
       <c r="J15">
-        <v>0.03530557407066226</v>
+        <v>0.04456278635188937</v>
       </c>
       <c r="K15">
-        <v>0.00816273083910346</v>
+        <v>0.007020831573754549</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1140,7 +1140,7 @@
         <v>4805</v>
       </c>
       <c r="E16">
-        <v>0.9390419572591782</v>
+        <v>1.19781486922875</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1154,28 +1154,28 @@
         <v>97</v>
       </c>
       <c r="D17">
-        <v>0.003192984033375978</v>
+        <v>0.002674760762602091</v>
       </c>
       <c r="E17">
-        <v>0.05968657089397311</v>
+        <v>0.05211486108601093</v>
       </c>
       <c r="F17">
         <v>97</v>
       </c>
       <c r="G17">
-        <v>0.004223072435706854</v>
+        <v>0.003274162299931049</v>
       </c>
       <c r="H17">
-        <v>0.03784104296937585</v>
+        <v>0.03258309187367558</v>
       </c>
       <c r="I17">
-        <v>0.001122236251831055</v>
+        <v>0.001271062064915895</v>
       </c>
       <c r="J17">
-        <v>0.01052592322230339</v>
+        <v>0.0103395851328969</v>
       </c>
       <c r="K17">
-        <v>0.001527272164821625</v>
+        <v>0.001199688762426376</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1187,28 +1187,28 @@
         <v>691</v>
       </c>
       <c r="D18">
-        <v>0.0009333062916994095</v>
+        <v>0.0008676475845277309</v>
       </c>
       <c r="E18">
-        <v>0.3100540842860937</v>
+        <v>0.3214176730252802</v>
       </c>
       <c r="F18">
         <v>691</v>
       </c>
       <c r="G18">
-        <v>0.02490810491144657</v>
+        <v>0.0224135834723711</v>
       </c>
       <c r="H18">
-        <v>0.2005890929140151</v>
+        <v>0.1991616445593536</v>
       </c>
       <c r="I18">
-        <v>0.0086867930367589</v>
+        <v>0.01742002135142684</v>
       </c>
       <c r="J18">
-        <v>0.03949838085100055</v>
+        <v>0.05026417504996061</v>
       </c>
       <c r="K18">
-        <v>0.008871165569871664</v>
+        <v>0.007777146995067596</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1220,28 +1220,28 @@
         <v>97</v>
       </c>
       <c r="D19">
-        <v>0.002967767417430878</v>
+        <v>0.002820469439029694</v>
       </c>
       <c r="E19">
-        <v>0.051557338796556</v>
+        <v>0.0530701931566</v>
       </c>
       <c r="F19">
         <v>97</v>
       </c>
       <c r="G19">
-        <v>0.003638145979493856</v>
+        <v>0.003372336272150278</v>
       </c>
       <c r="H19">
-        <v>0.03314039576798677</v>
+        <v>0.03259953297674656</v>
       </c>
       <c r="I19">
-        <v>0.00109127489849925</v>
+        <v>0.001340185292065144</v>
       </c>
       <c r="J19">
-        <v>0.008736977819353342</v>
+        <v>0.01092933863401413</v>
       </c>
       <c r="K19">
-        <v>0.001243905164301395</v>
+        <v>0.001208415254950523</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1253,28 +1253,28 @@
         <v>691</v>
       </c>
       <c r="D20">
-        <v>0.001468064729124308</v>
+        <v>0.001317867077887058</v>
       </c>
       <c r="E20">
-        <v>0.3119523008354008</v>
+        <v>0.3277451996691525</v>
       </c>
       <c r="F20">
         <v>691</v>
       </c>
       <c r="G20">
-        <v>0.02475325390696526</v>
+        <v>0.02273847255855799</v>
       </c>
       <c r="H20">
-        <v>0.2021430507302284</v>
+        <v>0.2024244735948741</v>
       </c>
       <c r="I20">
-        <v>0.009953280445188284</v>
+        <v>0.01867597969248891</v>
       </c>
       <c r="J20">
-        <v>0.03843353502452374</v>
+        <v>0.05149086331948638</v>
       </c>
       <c r="K20">
-        <v>0.008988030254840851</v>
+        <v>0.007962895557284355</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1286,7 +1286,7 @@
         <v>4805</v>
       </c>
       <c r="E21">
-        <v>0.9581344211474061</v>
+        <v>1.015661107841879</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1300,28 +1300,28 @@
         <v>80</v>
       </c>
       <c r="D22">
-        <v>0.002981758210808039</v>
+        <v>0.002665614243596792</v>
       </c>
       <c r="E22">
-        <v>0.05135160824283957</v>
+        <v>0.04612505994737148</v>
       </c>
       <c r="F22">
         <v>80</v>
       </c>
       <c r="G22">
-        <v>0.003661919850856066</v>
+        <v>0.002748556435108185</v>
       </c>
       <c r="H22">
-        <v>0.03342994069680572</v>
+        <v>0.02920609433203936</v>
       </c>
       <c r="I22">
-        <v>0.001056331675499678</v>
+        <v>0.00117412069812417</v>
       </c>
       <c r="J22">
-        <v>0.007929214742034674</v>
+        <v>0.009055460337549448</v>
       </c>
       <c r="K22">
-        <v>0.001306978985667229</v>
+        <v>0.001013088040053844</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1333,28 +1333,28 @@
         <v>645</v>
       </c>
       <c r="D23">
-        <v>0.0008408799767494202</v>
+        <v>0.0007669990882277489</v>
       </c>
       <c r="E23">
-        <v>0.2793110520578921</v>
+        <v>0.2942635361105204</v>
       </c>
       <c r="F23">
         <v>645</v>
       </c>
       <c r="G23">
-        <v>0.02277254359796643</v>
+        <v>0.02059155749157071</v>
       </c>
       <c r="H23">
-        <v>0.1806641155853868</v>
+        <v>0.1811021571047604</v>
       </c>
       <c r="I23">
-        <v>0.007609287276864052</v>
+        <v>0.0163769512437284</v>
       </c>
       <c r="J23">
-        <v>0.0350108789280057</v>
+        <v>0.04608120024204254</v>
       </c>
       <c r="K23">
-        <v>0.008100660517811775</v>
+        <v>0.007416658569127321</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1366,28 +1366,28 @@
         <v>80</v>
       </c>
       <c r="D24">
-        <v>0.002797433640807867</v>
+        <v>0.002863870933651924</v>
       </c>
       <c r="E24">
-        <v>0.04392475681379437</v>
+        <v>0.04482023511081934</v>
       </c>
       <c r="F24">
         <v>80</v>
       </c>
       <c r="G24">
-        <v>0.003027439117431641</v>
+        <v>0.002723724581301212</v>
       </c>
       <c r="H24">
-        <v>0.02779966033995152</v>
+        <v>0.02809604303911328</v>
       </c>
       <c r="I24">
-        <v>0.0009687785059213638</v>
+        <v>0.001164416316896677</v>
       </c>
       <c r="J24">
-        <v>0.007670196704566479</v>
+        <v>0.008978911675512791</v>
       </c>
       <c r="K24">
-        <v>0.001151410862803459</v>
+        <v>0.0009899823926389217</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1399,28 +1399,28 @@
         <v>645</v>
       </c>
       <c r="D25">
-        <v>0.001083121635019779</v>
+        <v>0.001167423091828823</v>
       </c>
       <c r="E25">
-        <v>0.2651075110770762</v>
+        <v>0.3058887221850455</v>
       </c>
       <c r="F25">
         <v>645</v>
       </c>
       <c r="G25">
-        <v>0.02058612275868654</v>
+        <v>0.02149605099111795</v>
       </c>
       <c r="H25">
-        <v>0.1708462117239833</v>
+        <v>0.1878059906885028</v>
       </c>
       <c r="I25">
-        <v>0.008810519706457853</v>
+        <v>0.0177012630738318</v>
       </c>
       <c r="J25">
-        <v>0.0340973143465817</v>
+        <v>0.04820545297116041</v>
       </c>
       <c r="K25">
-        <v>0.007779397536069155</v>
+        <v>0.007510603405535221</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1432,7 +1432,7 @@
         <v>4805</v>
       </c>
       <c r="E26">
-        <v>1.1352184927091</v>
+        <v>1.154503941070288</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1446,28 +1446,28 @@
         <v>84.8</v>
       </c>
       <c r="D27">
-        <v>0.004420891217887401</v>
+        <v>0.003205010294914246</v>
       </c>
       <c r="E27">
-        <v>0.06838358081877231</v>
+        <v>0.05502571165561676</v>
       </c>
       <c r="F27">
         <v>84.8</v>
       </c>
       <c r="G27">
-        <v>0.004853783547878266</v>
+        <v>0.003396784700453281</v>
       </c>
       <c r="H27">
-        <v>0.04416513368487358</v>
+        <v>0.03465584823861718</v>
       </c>
       <c r="I27">
-        <v>0.001439846213907003</v>
+        <v>0.001489860843867063</v>
       </c>
       <c r="J27">
-        <v>0.01114206705242395</v>
+        <v>0.0106443946249783</v>
       </c>
       <c r="K27">
-        <v>0.001664528157562017</v>
+        <v>0.001247777696698904</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1479,28 +1479,28 @@
         <v>695.6</v>
       </c>
       <c r="D28">
-        <v>0.0009116794914007187</v>
+        <v>0.0008684741333127022</v>
       </c>
       <c r="E28">
-        <v>0.3026251026429236</v>
+        <v>0.3269761184230447</v>
       </c>
       <c r="F28">
         <v>695.6</v>
       </c>
       <c r="G28">
-        <v>0.02434277851134539</v>
+        <v>0.02291050618514419</v>
       </c>
       <c r="H28">
-        <v>0.1952384945005178</v>
+        <v>0.2028767012059688</v>
       </c>
       <c r="I28">
-        <v>0.008333943039178848</v>
+        <v>0.01711173020303249</v>
       </c>
       <c r="J28">
-        <v>0.03909624628722667</v>
+        <v>0.05115713430568576</v>
       </c>
       <c r="K28">
-        <v>0.008723151218146086</v>
+        <v>0.007992563024163245</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1512,28 +1512,28 @@
         <v>84.8</v>
       </c>
       <c r="D29">
-        <v>0.004775155801326036</v>
+        <v>0.00344582675024867</v>
       </c>
       <c r="E29">
-        <v>0.07322538066655397</v>
+        <v>0.0562193913385272</v>
       </c>
       <c r="F29">
         <v>84.8</v>
       </c>
       <c r="G29">
-        <v>0.005045556835830212</v>
+        <v>0.003517439868301153</v>
       </c>
       <c r="H29">
-        <v>0.04735847292467952</v>
+        <v>0.03530614804476499</v>
       </c>
       <c r="I29">
-        <v>0.001557187363505363</v>
+        <v>0.001508807856589556</v>
       </c>
       <c r="J29">
-        <v>0.01199029972776771</v>
+        <v>0.01091162376105785</v>
       </c>
       <c r="K29">
-        <v>0.001813339814543724</v>
+        <v>0.001240631192922592</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1545,28 +1545,28 @@
         <v>695.6</v>
       </c>
       <c r="D30">
-        <v>0.001401296630501747</v>
+        <v>0.001292264834046364</v>
       </c>
       <c r="E30">
-        <v>0.3236090023070574</v>
+        <v>0.3311198697425425</v>
       </c>
       <c r="F30">
         <v>695.6</v>
       </c>
       <c r="G30">
-        <v>0.02546346820890904</v>
+        <v>0.02334131486713886</v>
       </c>
       <c r="H30">
-        <v>0.209005671646446</v>
+        <v>0.2046307132579386</v>
       </c>
       <c r="I30">
-        <v>0.01057074591517448</v>
+        <v>0.01818280899897218</v>
       </c>
       <c r="J30">
-        <v>0.0407187519595027</v>
+        <v>0.05179475480690598</v>
       </c>
       <c r="K30">
-        <v>0.009383930545300245</v>
+        <v>0.008085385710000993</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1578,7 +1578,7 @@
         <v>4805</v>
       </c>
       <c r="E31">
-        <v>0.9698823684826493</v>
+        <v>1.064235171861946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nearly passing all tests, except xcept . Seems that global bound must be a function of path criteria
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -716,28 +716,28 @@
         <v>103</v>
       </c>
       <c r="D2">
-        <v>0.004212758503854275</v>
+        <v>0.003961923997849226</v>
       </c>
       <c r="E2">
-        <v>0.0673017748631537</v>
+        <v>0.06242087110877037</v>
       </c>
       <c r="F2">
         <v>103</v>
       </c>
       <c r="G2">
-        <v>0.004141566343605518</v>
+        <v>0.004758586175739765</v>
       </c>
       <c r="H2">
-        <v>0.04282997362315655</v>
+        <v>0.03974230634048581</v>
       </c>
       <c r="I2">
-        <v>0.001827794127166271</v>
+        <v>0.001530169509351254</v>
       </c>
       <c r="J2">
-        <v>0.01286618737503886</v>
+        <v>0.009129321202635765</v>
       </c>
       <c r="K2">
-        <v>0.001410416327416897</v>
+        <v>0.00285257725045085</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -749,28 +749,28 @@
         <v>841</v>
       </c>
       <c r="D3">
-        <v>0.001007826998829842</v>
+        <v>0.002390699461102486</v>
       </c>
       <c r="E3">
-        <v>0.3842693129554391</v>
+        <v>0.3609774098731577</v>
       </c>
       <c r="F3">
         <v>841</v>
       </c>
       <c r="G3">
-        <v>0.02702527865767479</v>
+        <v>0.03056043619289994</v>
       </c>
       <c r="H3">
-        <v>0.2381146480329335</v>
+        <v>0.22402598336339</v>
       </c>
       <c r="I3">
-        <v>0.01914155157282948</v>
+        <v>0.01802518498152494</v>
       </c>
       <c r="J3">
-        <v>0.06134908180683851</v>
+        <v>0.04083840968087316</v>
       </c>
       <c r="K3">
-        <v>0.009389501065015793</v>
+        <v>0.01866521127521992</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -782,28 +782,28 @@
         <v>103</v>
       </c>
       <c r="D4">
-        <v>0.004408972337841988</v>
+        <v>0.003317888826131821</v>
       </c>
       <c r="E4">
-        <v>0.06654203357174993</v>
+        <v>0.05858613131567836</v>
       </c>
       <c r="F4">
         <v>103</v>
       </c>
       <c r="G4">
-        <v>0.004251713398844004</v>
+        <v>0.004581920802593231</v>
       </c>
       <c r="H4">
-        <v>0.04214417422190309</v>
+        <v>0.03666938655078411</v>
       </c>
       <c r="I4">
-        <v>0.001718732062727213</v>
+        <v>0.001605357509106398</v>
       </c>
       <c r="J4">
-        <v>0.01264319103211164</v>
+        <v>0.009125441778451204</v>
       </c>
       <c r="K4">
-        <v>0.001474219374358654</v>
+        <v>0.002569119445979595</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -815,28 +815,28 @@
         <v>841</v>
       </c>
       <c r="D5">
-        <v>0.001479329541325569</v>
+        <v>0.00149089377373457</v>
       </c>
       <c r="E5">
-        <v>0.383428439963609</v>
+        <v>0.3604000369086862</v>
       </c>
       <c r="F5">
         <v>841</v>
       </c>
       <c r="G5">
-        <v>0.02749304007738829</v>
+        <v>0.03053943580016494</v>
       </c>
       <c r="H5">
-        <v>0.2364881676621735</v>
+        <v>0.2217852910980582</v>
       </c>
       <c r="I5">
-        <v>0.0199749581515789</v>
+        <v>0.01878394279628992</v>
       </c>
       <c r="J5">
-        <v>0.06070742849260569</v>
+        <v>0.04089313978329301</v>
       </c>
       <c r="K5">
-        <v>0.009437066502869129</v>
+        <v>0.01894107880070806</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -845,10 +845,10 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1.035875022411346</v>
+        <v>1.106505824718624</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -862,28 +862,28 @@
         <v>59</v>
       </c>
       <c r="D7">
-        <v>0.004190638661384583</v>
+        <v>0.002617233898490667</v>
       </c>
       <c r="E7">
-        <v>0.06552575435489416</v>
+        <v>0.03924175398424268</v>
       </c>
       <c r="F7">
         <v>59</v>
       </c>
       <c r="G7">
-        <v>0.004033647943288088</v>
+        <v>0.002862686756998301</v>
       </c>
       <c r="H7">
-        <v>0.04086672281846404</v>
+        <v>0.02421921771019697</v>
       </c>
       <c r="I7">
-        <v>0.00188658619299531</v>
+        <v>0.001118030864745378</v>
       </c>
       <c r="J7">
-        <v>0.01274234103038907</v>
+        <v>0.006645085755735636</v>
       </c>
       <c r="K7">
-        <v>0.001625906210392714</v>
+        <v>0.001754528842866421</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -895,28 +895,28 @@
         <v>684</v>
       </c>
       <c r="D8">
-        <v>0.0009196139872074127</v>
+        <v>0.002056588884443045</v>
       </c>
       <c r="E8">
-        <v>0.3518870892003179</v>
+        <v>0.305586124304682</v>
       </c>
       <c r="F8">
         <v>684</v>
       </c>
       <c r="G8">
-        <v>0.02473711036145687</v>
+        <v>0.02601653430610895</v>
       </c>
       <c r="H8">
-        <v>0.2196963313035667</v>
+        <v>0.1881138212047517</v>
       </c>
       <c r="I8">
-        <v>0.01750291045755148</v>
+        <v>0.01473014336079359</v>
       </c>
       <c r="J8">
-        <v>0.05480776494368911</v>
+        <v>0.03534559765830636</v>
       </c>
       <c r="K8">
-        <v>0.008440659381449223</v>
+        <v>0.01616413472220302</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -928,28 +928,28 @@
         <v>59</v>
       </c>
       <c r="D9">
-        <v>0.004432704299688339</v>
+        <v>0.002436739392578602</v>
       </c>
       <c r="E9">
-        <v>0.06589768594130874</v>
+        <v>0.03652191301807761</v>
       </c>
       <c r="F9">
         <v>59</v>
       </c>
       <c r="G9">
-        <v>0.004031843040138483</v>
+        <v>0.00274158688262105</v>
       </c>
       <c r="H9">
-        <v>0.04140257462859154</v>
+        <v>0.02291522035375237</v>
       </c>
       <c r="I9">
-        <v>0.001947587821632624</v>
+        <v>0.001087508164346218</v>
       </c>
       <c r="J9">
-        <v>0.01288035791367292</v>
+        <v>0.005839633289724588</v>
       </c>
       <c r="K9">
-        <v>0.001401062123477459</v>
+        <v>0.001547982916235924</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -961,28 +961,28 @@
         <v>684</v>
       </c>
       <c r="D10">
-        <v>0.001342307776212692</v>
+        <v>0.001243194565176964</v>
       </c>
       <c r="E10">
-        <v>0.3479090337641537</v>
+        <v>0.2937803077511489</v>
       </c>
       <c r="F10">
         <v>684</v>
       </c>
       <c r="G10">
-        <v>0.02436545863747597</v>
+        <v>0.02501813694834709</v>
       </c>
       <c r="H10">
-        <v>0.2163986614905298</v>
+        <v>0.1808811011724174</v>
       </c>
       <c r="I10">
-        <v>0.01830550003796816</v>
+        <v>0.0151786208152771</v>
       </c>
       <c r="J10">
-        <v>0.05400724289938807</v>
+        <v>0.03359454357996583</v>
       </c>
       <c r="K10">
-        <v>0.008495531510561705</v>
+        <v>0.01547997817397118</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -991,10 +991,10 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.9173209187574685</v>
+        <v>0.8979644482024014</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1008,28 +1008,28 @@
         <v>85</v>
       </c>
       <c r="D12">
-        <v>0.002281279303133488</v>
+        <v>0.002382888458669186</v>
       </c>
       <c r="E12">
-        <v>0.04406110802665353</v>
+        <v>0.04156492277979851</v>
       </c>
       <c r="F12">
         <v>85</v>
       </c>
       <c r="G12">
-        <v>0.002785990480333567</v>
+        <v>0.00315969018265605</v>
       </c>
       <c r="H12">
-        <v>0.02779335854575038</v>
+        <v>0.0261453534476459</v>
       </c>
       <c r="I12">
-        <v>0.001289741136133671</v>
+        <v>0.001290869433432817</v>
       </c>
       <c r="J12">
-        <v>0.008218399249017239</v>
+        <v>0.006088669877499342</v>
       </c>
       <c r="K12">
-        <v>0.000989789143204689</v>
+        <v>0.001958401873707771</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1041,28 +1041,28 @@
         <v>617</v>
       </c>
       <c r="D13">
-        <v>0.0007802830077707767</v>
+        <v>0.001847608014941216</v>
       </c>
       <c r="E13">
-        <v>0.2830429808236659</v>
+        <v>0.2679000240750611</v>
       </c>
       <c r="F13">
         <v>617</v>
       </c>
       <c r="G13">
-        <v>0.01978500094264746</v>
+        <v>0.0221830909140408</v>
       </c>
       <c r="H13">
-        <v>0.1763087250292301</v>
+        <v>0.1667156340554357</v>
       </c>
       <c r="I13">
-        <v>0.01511721638962626</v>
+        <v>0.01391408080235124</v>
       </c>
       <c r="J13">
-        <v>0.04328344948589802</v>
+        <v>0.02962920162826777</v>
       </c>
       <c r="K13">
-        <v>0.006938849110156298</v>
+        <v>0.01398213813081384</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1074,28 +1074,28 @@
         <v>85</v>
       </c>
       <c r="D14">
-        <v>0.002703116741031408</v>
+        <v>0.002360836137086153</v>
       </c>
       <c r="E14">
-        <v>0.05076680891215801</v>
+        <v>0.04394010920077562</v>
       </c>
       <c r="F14">
         <v>85</v>
       </c>
       <c r="G14">
-        <v>0.003207582049071789</v>
+        <v>0.003344262484461069</v>
       </c>
       <c r="H14">
-        <v>0.03228841535747051</v>
+        <v>0.0275275120511651</v>
       </c>
       <c r="I14">
-        <v>0.001373117789626122</v>
+        <v>0.001386471092700958</v>
       </c>
       <c r="J14">
-        <v>0.009126319549977779</v>
+        <v>0.00632206117734313</v>
       </c>
       <c r="K14">
-        <v>0.001129476819187403</v>
+        <v>0.002075059805065393</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1107,28 +1107,28 @@
         <v>617</v>
       </c>
       <c r="D15">
-        <v>0.001154396682977676</v>
+        <v>0.001198198180645704</v>
       </c>
       <c r="E15">
-        <v>0.2906279531307518</v>
+        <v>0.2847359217703342</v>
       </c>
       <c r="F15">
         <v>617</v>
       </c>
       <c r="G15">
-        <v>0.02061355207115412</v>
+        <v>0.02414836501702666</v>
       </c>
       <c r="H15">
-        <v>0.1800362728536129</v>
+        <v>0.1748937289230525</v>
       </c>
       <c r="I15">
-        <v>0.01625634403899312</v>
+        <v>0.01591190975159407</v>
       </c>
       <c r="J15">
-        <v>0.04456278635188937</v>
+        <v>0.03171652369201183</v>
       </c>
       <c r="K15">
-        <v>0.007020831573754549</v>
+        <v>0.01497953571379185</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1137,10 +1137,10 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1.19781486922875</v>
+        <v>1.059409182518721</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1154,28 +1154,28 @@
         <v>97</v>
       </c>
       <c r="D17">
-        <v>0.002674760762602091</v>
+        <v>0.002766044810414314</v>
       </c>
       <c r="E17">
-        <v>0.05211486108601093</v>
+        <v>0.05008273618295789</v>
       </c>
       <c r="F17">
         <v>97</v>
       </c>
       <c r="G17">
-        <v>0.003274162299931049</v>
+        <v>0.003728274255990982</v>
       </c>
       <c r="H17">
-        <v>0.03258309187367558</v>
+        <v>0.03120582643896341</v>
       </c>
       <c r="I17">
-        <v>0.001271062064915895</v>
+        <v>0.001357139553874731</v>
       </c>
       <c r="J17">
-        <v>0.0103395851328969</v>
+        <v>0.007799938321113586</v>
       </c>
       <c r="K17">
-        <v>0.001199688762426376</v>
+        <v>0.00234952662140131</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1187,28 +1187,28 @@
         <v>691</v>
       </c>
       <c r="D18">
-        <v>0.0008676475845277309</v>
+        <v>0.002069283742457628</v>
       </c>
       <c r="E18">
-        <v>0.3214176730252802</v>
+        <v>0.3067218810319901</v>
       </c>
       <c r="F18">
         <v>691</v>
       </c>
       <c r="G18">
-        <v>0.0224135834723711</v>
+        <v>0.02578407153487206</v>
       </c>
       <c r="H18">
-        <v>0.1991616445593536</v>
+        <v>0.1884060804732144</v>
       </c>
       <c r="I18">
-        <v>0.01742002135142684</v>
+        <v>0.01634280104190111</v>
       </c>
       <c r="J18">
-        <v>0.05026417504996061</v>
+        <v>0.03542019426822662</v>
       </c>
       <c r="K18">
-        <v>0.007777146995067596</v>
+        <v>0.01606227504089475</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1220,28 +1220,28 @@
         <v>97</v>
       </c>
       <c r="D19">
-        <v>0.002820469439029694</v>
+        <v>0.00293141882866621</v>
       </c>
       <c r="E19">
-        <v>0.0530701931566</v>
+        <v>0.05188515409827232</v>
       </c>
       <c r="F19">
         <v>97</v>
       </c>
       <c r="G19">
-        <v>0.003372336272150278</v>
+        <v>0.00397630175575614</v>
       </c>
       <c r="H19">
-        <v>0.03259953297674656</v>
+        <v>0.03239032998681068</v>
       </c>
       <c r="I19">
-        <v>0.001340185292065144</v>
+        <v>0.001482035033404827</v>
       </c>
       <c r="J19">
-        <v>0.01092933863401413</v>
+        <v>0.008001338224858046</v>
       </c>
       <c r="K19">
-        <v>0.001208415254950523</v>
+        <v>0.002349940128624439</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1253,28 +1253,28 @@
         <v>691</v>
       </c>
       <c r="D20">
-        <v>0.001317867077887058</v>
+        <v>0.001264994964003563</v>
       </c>
       <c r="E20">
-        <v>0.3277451996691525</v>
+        <v>0.300749619025737</v>
       </c>
       <c r="F20">
         <v>691</v>
       </c>
       <c r="G20">
-        <v>0.02273847255855799</v>
+        <v>0.0252198320813477</v>
       </c>
       <c r="H20">
-        <v>0.2024244735948741</v>
+        <v>0.1854279190301895</v>
       </c>
       <c r="I20">
-        <v>0.01867597969248891</v>
+        <v>0.01708532124757767</v>
       </c>
       <c r="J20">
-        <v>0.05149086331948638</v>
+        <v>0.03404026012867689</v>
       </c>
       <c r="K20">
-        <v>0.007962895557284355</v>
+        <v>0.01527096331119537</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1283,10 +1283,10 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1.015661107841879</v>
+        <v>1.00795480562374</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1300,28 +1300,28 @@
         <v>80</v>
       </c>
       <c r="D22">
-        <v>0.002665614243596792</v>
+        <v>0.002676998730748892</v>
       </c>
       <c r="E22">
-        <v>0.04612505994737148</v>
+        <v>0.04325457895174623</v>
       </c>
       <c r="F22">
         <v>80</v>
       </c>
       <c r="G22">
-        <v>0.002748556435108185</v>
+        <v>0.003306585364043713</v>
       </c>
       <c r="H22">
-        <v>0.02920609433203936</v>
+        <v>0.02701234305277467</v>
       </c>
       <c r="I22">
-        <v>0.00117412069812417</v>
+        <v>0.00129800708964467</v>
       </c>
       <c r="J22">
-        <v>0.009055460337549448</v>
+        <v>0.006706702057272196</v>
       </c>
       <c r="K22">
-        <v>0.001013088040053844</v>
+        <v>0.001983508002012968</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1333,28 +1333,28 @@
         <v>645</v>
       </c>
       <c r="D23">
-        <v>0.0007669990882277489</v>
+        <v>0.001876875292509794</v>
       </c>
       <c r="E23">
-        <v>0.2942635361105204</v>
+        <v>0.2856964897364378</v>
       </c>
       <c r="F23">
         <v>645</v>
       </c>
       <c r="G23">
-        <v>0.02059155749157071</v>
+        <v>0.02377653401345015</v>
       </c>
       <c r="H23">
-        <v>0.1811021571047604</v>
+        <v>0.1768475039862096</v>
       </c>
       <c r="I23">
-        <v>0.0163769512437284</v>
+        <v>0.01542425900697708</v>
       </c>
       <c r="J23">
-        <v>0.04608120024204254</v>
+        <v>0.0322994259186089</v>
       </c>
       <c r="K23">
-        <v>0.007416658569127321</v>
+        <v>0.01486537978053093</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1366,28 +1366,28 @@
         <v>80</v>
       </c>
       <c r="D24">
-        <v>0.002863870933651924</v>
+        <v>0.002617469057440758</v>
       </c>
       <c r="E24">
-        <v>0.04482023511081934</v>
+        <v>0.04459123313426971</v>
       </c>
       <c r="F24">
         <v>80</v>
       </c>
       <c r="G24">
-        <v>0.002723724581301212</v>
+        <v>0.003365387208759785</v>
       </c>
       <c r="H24">
-        <v>0.02809604303911328</v>
+        <v>0.0278595769777894</v>
       </c>
       <c r="I24">
-        <v>0.001164416316896677</v>
+        <v>0.001256630290299654</v>
       </c>
       <c r="J24">
-        <v>0.008978911675512791</v>
+        <v>0.006917370017617941</v>
       </c>
       <c r="K24">
-        <v>0.0009899823926389217</v>
+        <v>0.002033184748142958</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1399,28 +1399,28 @@
         <v>645</v>
       </c>
       <c r="D25">
-        <v>0.001167423091828823</v>
+        <v>0.00120099913328886</v>
       </c>
       <c r="E25">
-        <v>0.3058887221850455</v>
+        <v>0.2911525252275169</v>
       </c>
       <c r="F25">
         <v>645</v>
       </c>
       <c r="G25">
-        <v>0.02149605099111795</v>
+        <v>0.02450546575710177</v>
       </c>
       <c r="H25">
-        <v>0.1878059906885028</v>
+        <v>0.178148933686316</v>
       </c>
       <c r="I25">
-        <v>0.0177012630738318</v>
+        <v>0.01639682101085782</v>
       </c>
       <c r="J25">
-        <v>0.04820545297116041</v>
+        <v>0.03340143710374832</v>
       </c>
       <c r="K25">
-        <v>0.007510603405535221</v>
+        <v>0.0150182475335896</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1429,10 +1429,10 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1.154503941070288</v>
+        <v>0.8913419921882451</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1446,28 +1446,28 @@
         <v>84.8</v>
       </c>
       <c r="D27">
-        <v>0.003205010294914246</v>
+        <v>0.002881017979234457</v>
       </c>
       <c r="E27">
-        <v>0.05502571165561676</v>
+        <v>0.04731297260150313</v>
       </c>
       <c r="F27">
         <v>84.8</v>
       </c>
       <c r="G27">
-        <v>0.003396784700453281</v>
+        <v>0.003563164547085762</v>
       </c>
       <c r="H27">
-        <v>0.03465584823861718</v>
+        <v>0.02966500939801335</v>
       </c>
       <c r="I27">
-        <v>0.001489860843867063</v>
+        <v>0.00131884329020977</v>
       </c>
       <c r="J27">
-        <v>0.0106443946249783</v>
+        <v>0.007273943442851305</v>
       </c>
       <c r="K27">
-        <v>0.001247777696698904</v>
+        <v>0.002179708518087864</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1479,28 +1479,28 @@
         <v>695.6</v>
       </c>
       <c r="D28">
-        <v>0.0008684741333127022</v>
+        <v>0.002048211079090834</v>
       </c>
       <c r="E28">
-        <v>0.3269761184230447</v>
+        <v>0.3053763858042657</v>
       </c>
       <c r="F28">
         <v>695.6</v>
       </c>
       <c r="G28">
-        <v>0.02291050618514419</v>
+        <v>0.02566413339227438</v>
       </c>
       <c r="H28">
-        <v>0.2028767012059688</v>
+        <v>0.1888218046166003</v>
       </c>
       <c r="I28">
-        <v>0.01711173020303249</v>
+        <v>0.01568729383870959</v>
       </c>
       <c r="J28">
-        <v>0.05115713430568576</v>
+        <v>0.03470656583085656</v>
       </c>
       <c r="K28">
-        <v>0.007992563024163245</v>
+        <v>0.01594782778993249</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1512,28 +1512,28 @@
         <v>84.8</v>
       </c>
       <c r="D29">
-        <v>0.00344582675024867</v>
+        <v>0.002732870448380709</v>
       </c>
       <c r="E29">
-        <v>0.0562193913385272</v>
+        <v>0.04710490815341473</v>
       </c>
       <c r="F29">
         <v>84.8</v>
       </c>
       <c r="G29">
-        <v>0.003517439868301153</v>
+        <v>0.003601891826838255</v>
       </c>
       <c r="H29">
-        <v>0.03530614804476499</v>
+        <v>0.02947240518406034</v>
       </c>
       <c r="I29">
-        <v>0.001508807856589556</v>
+        <v>0.001363600417971611</v>
       </c>
       <c r="J29">
-        <v>0.01091162376105785</v>
+        <v>0.007241168897598982</v>
       </c>
       <c r="K29">
-        <v>0.001240631192922592</v>
+        <v>0.002115057408809662</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1545,28 +1545,28 @@
         <v>695.6</v>
       </c>
       <c r="D30">
-        <v>0.001292264834046364</v>
+        <v>0.001279656123369932</v>
       </c>
       <c r="E30">
-        <v>0.3311198697425425</v>
+        <v>0.3061636821366847</v>
       </c>
       <c r="F30">
         <v>695.6</v>
       </c>
       <c r="G30">
-        <v>0.02334131486713886</v>
+        <v>0.02588624712079763</v>
       </c>
       <c r="H30">
-        <v>0.2046307132579386</v>
+        <v>0.1882273947820067</v>
       </c>
       <c r="I30">
-        <v>0.01818280899897218</v>
+        <v>0.01667132312431931</v>
       </c>
       <c r="J30">
-        <v>0.05179475480690598</v>
+        <v>0.03472918085753918</v>
       </c>
       <c r="K30">
-        <v>0.008085385710000993</v>
+        <v>0.01593796070665121</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1575,10 +1575,10 @@
         <v>25</v>
       </c>
       <c r="C31">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1.064235171861946</v>
+        <v>0.9926352506503463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating version to 2 see changelog
</commit_message>
<xml_diff>
--- a/tests/advanced/processed_all_results_test.xlsx
+++ b/tests/advanced/processed_all_results_test.xlsx
@@ -716,28 +716,28 @@
         <v>103</v>
       </c>
       <c r="D2">
-        <v>0.003961923997849226</v>
+        <v>0.005102754570543766</v>
       </c>
       <c r="E2">
-        <v>0.06242087110877037</v>
+        <v>0.08766797697171569</v>
       </c>
       <c r="F2">
         <v>103</v>
       </c>
       <c r="G2">
-        <v>0.004758586175739765</v>
+        <v>0.00647373590618372</v>
       </c>
       <c r="H2">
-        <v>0.03974230634048581</v>
+        <v>0.05529298214241862</v>
       </c>
       <c r="I2">
-        <v>0.001530169509351254</v>
+        <v>0.002181593794375658</v>
       </c>
       <c r="J2">
-        <v>0.009129321202635765</v>
+        <v>0.01306318817660213</v>
       </c>
       <c r="K2">
-        <v>0.00285257725045085</v>
+        <v>0.004212494008243084</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -749,28 +749,28 @@
         <v>841</v>
       </c>
       <c r="D3">
-        <v>0.002390699461102486</v>
+        <v>0.002768766600638628</v>
       </c>
       <c r="E3">
-        <v>0.3609774098731577</v>
+        <v>0.3978188671171665</v>
       </c>
       <c r="F3">
         <v>841</v>
       </c>
       <c r="G3">
-        <v>0.03056043619289994</v>
+        <v>0.0329343150369823</v>
       </c>
       <c r="H3">
-        <v>0.22402598336339</v>
+        <v>0.2477840362116694</v>
       </c>
       <c r="I3">
-        <v>0.01802518498152494</v>
+        <v>0.02008050912991166</v>
       </c>
       <c r="J3">
-        <v>0.04083840968087316</v>
+        <v>0.04348715161904693</v>
       </c>
       <c r="K3">
-        <v>0.01866521127521992</v>
+        <v>0.02110619191080332</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -782,28 +782,28 @@
         <v>103</v>
       </c>
       <c r="D4">
-        <v>0.003317888826131821</v>
+        <v>0.004544228781014681</v>
       </c>
       <c r="E4">
-        <v>0.05858613131567836</v>
+        <v>0.08951445901766419</v>
       </c>
       <c r="F4">
         <v>103</v>
       </c>
       <c r="G4">
-        <v>0.004581920802593231</v>
+        <v>0.00708110723644495</v>
       </c>
       <c r="H4">
-        <v>0.03666938655078411</v>
+        <v>0.05620518606156111</v>
       </c>
       <c r="I4">
-        <v>0.001605357509106398</v>
+        <v>0.002070061396807432</v>
       </c>
       <c r="J4">
-        <v>0.009125441778451204</v>
+        <v>0.01354377809911966</v>
       </c>
       <c r="K4">
-        <v>0.002569119445979595</v>
+        <v>0.004198172129690647</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -815,28 +815,28 @@
         <v>841</v>
       </c>
       <c r="D5">
-        <v>0.00149089377373457</v>
+        <v>0.00162486732006073</v>
       </c>
       <c r="E5">
-        <v>0.3604000369086862</v>
+        <v>0.3988577299751341</v>
       </c>
       <c r="F5">
         <v>841</v>
       </c>
       <c r="G5">
-        <v>0.03053943580016494</v>
+        <v>0.03452201280742884</v>
       </c>
       <c r="H5">
-        <v>0.2217852910980582</v>
+        <v>0.2477879533544183</v>
       </c>
       <c r="I5">
-        <v>0.01878394279628992</v>
+        <v>0.02027707872912288</v>
       </c>
       <c r="J5">
-        <v>0.04089313978329301</v>
+        <v>0.0441118972375989</v>
       </c>
       <c r="K5">
-        <v>0.01894107880070806</v>
+        <v>0.02071312442421913</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -845,10 +845,10 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4805</v>
       </c>
       <c r="E6">
-        <v>1.106505824718624</v>
+        <v>1.298504695296288</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -862,28 +862,28 @@
         <v>59</v>
       </c>
       <c r="D7">
-        <v>0.002617233898490667</v>
+        <v>0.002298991661518812</v>
       </c>
       <c r="E7">
-        <v>0.03924175398424268</v>
+        <v>0.03687652293592691</v>
       </c>
       <c r="F7">
         <v>59</v>
       </c>
       <c r="G7">
-        <v>0.002862686756998301</v>
+        <v>0.002486546989530325</v>
       </c>
       <c r="H7">
-        <v>0.02421921771019697</v>
+        <v>0.02200968703255057</v>
       </c>
       <c r="I7">
-        <v>0.001118030864745378</v>
+        <v>0.001150201074779034</v>
       </c>
       <c r="J7">
-        <v>0.006645085755735636</v>
+        <v>0.007398577872663736</v>
       </c>
       <c r="K7">
-        <v>0.001754528842866421</v>
+        <v>0.00150013854727149</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -895,28 +895,28 @@
         <v>684</v>
       </c>
       <c r="D8">
-        <v>0.002056588884443045</v>
+        <v>0.002187779173254967</v>
       </c>
       <c r="E8">
-        <v>0.305586124304682</v>
+        <v>0.3089819452725351</v>
       </c>
       <c r="F8">
         <v>684</v>
       </c>
       <c r="G8">
-        <v>0.02601653430610895</v>
+        <v>0.02513412712141871</v>
       </c>
       <c r="H8">
-        <v>0.1881138212047517</v>
+        <v>0.1923001850955188</v>
       </c>
       <c r="I8">
-        <v>0.01473014336079359</v>
+        <v>0.01554499007761478</v>
       </c>
       <c r="J8">
-        <v>0.03534559765830636</v>
+        <v>0.03539645997807384</v>
       </c>
       <c r="K8">
-        <v>0.01616413472220302</v>
+        <v>0.01592940557748079</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -928,28 +928,28 @@
         <v>59</v>
       </c>
       <c r="D9">
-        <v>0.002436739392578602</v>
+        <v>0.002204176038503647</v>
       </c>
       <c r="E9">
-        <v>0.03652191301807761</v>
+        <v>0.03687581699341536</v>
       </c>
       <c r="F9">
         <v>59</v>
       </c>
       <c r="G9">
-        <v>0.00274158688262105</v>
+        <v>0.00262652151286602</v>
       </c>
       <c r="H9">
-        <v>0.02291522035375237</v>
+        <v>0.02256414387375116</v>
       </c>
       <c r="I9">
-        <v>0.001087508164346218</v>
+        <v>0.001185137778520584</v>
       </c>
       <c r="J9">
-        <v>0.005839633289724588</v>
+        <v>0.006533857434988022</v>
       </c>
       <c r="K9">
-        <v>0.001547982916235924</v>
+        <v>0.00162496929988265</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -961,28 +961,28 @@
         <v>684</v>
       </c>
       <c r="D10">
-        <v>0.001243194565176964</v>
+        <v>0.00132397934794426</v>
       </c>
       <c r="E10">
-        <v>0.2937803077511489</v>
+        <v>0.3183064819313586</v>
       </c>
       <c r="F10">
         <v>684</v>
       </c>
       <c r="G10">
-        <v>0.02501813694834709</v>
+        <v>0.02731511415913701</v>
       </c>
       <c r="H10">
-        <v>0.1808811011724174</v>
+        <v>0.1957804700359702</v>
       </c>
       <c r="I10">
-        <v>0.0151786208152771</v>
+        <v>0.01657566009089351</v>
       </c>
       <c r="J10">
-        <v>0.03359454357996583</v>
+        <v>0.03699039248749614</v>
       </c>
       <c r="K10">
-        <v>0.01547997817397118</v>
+        <v>0.01647298689931631</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -991,10 +991,10 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>4805</v>
       </c>
       <c r="E11">
-        <v>0.8979644482024014</v>
+        <v>1.028471729718149</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1008,28 +1008,28 @@
         <v>85</v>
       </c>
       <c r="D12">
-        <v>0.002382888458669186</v>
+        <v>0.002532277256250381</v>
       </c>
       <c r="E12">
-        <v>0.04156492277979851</v>
+        <v>0.04274594411253929</v>
       </c>
       <c r="F12">
         <v>85</v>
       </c>
       <c r="G12">
-        <v>0.00315969018265605</v>
+        <v>0.003110010176897049</v>
       </c>
       <c r="H12">
-        <v>0.0261453534476459</v>
+        <v>0.02715241070836782</v>
       </c>
       <c r="I12">
-        <v>0.001290869433432817</v>
+        <v>0.001401375513523817</v>
       </c>
       <c r="J12">
-        <v>0.006088669877499342</v>
+        <v>0.006053993478417397</v>
       </c>
       <c r="K12">
-        <v>0.001958401873707771</v>
+        <v>0.001905275508761406</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1041,28 +1041,28 @@
         <v>617</v>
       </c>
       <c r="D13">
-        <v>0.001847608014941216</v>
+        <v>0.001971160061657429</v>
       </c>
       <c r="E13">
-        <v>0.2679000240750611</v>
+        <v>0.2753048120066524</v>
       </c>
       <c r="F13">
         <v>617</v>
       </c>
       <c r="G13">
-        <v>0.0221830909140408</v>
+        <v>0.02226255927234888</v>
       </c>
       <c r="H13">
-        <v>0.1667156340554357</v>
+        <v>0.1715072728693485</v>
       </c>
       <c r="I13">
-        <v>0.01391408080235124</v>
+        <v>0.01504562515765429</v>
       </c>
       <c r="J13">
-        <v>0.02962920162826777</v>
+        <v>0.03031315561383963</v>
       </c>
       <c r="K13">
-        <v>0.01398213813081384</v>
+        <v>0.01421913085505366</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1074,28 +1074,28 @@
         <v>85</v>
       </c>
       <c r="D14">
-        <v>0.002360836137086153</v>
+        <v>0.002352155745029449</v>
       </c>
       <c r="E14">
-        <v>0.04394010920077562</v>
+        <v>0.04351937724277377</v>
       </c>
       <c r="F14">
         <v>85</v>
       </c>
       <c r="G14">
-        <v>0.003344262484461069</v>
+        <v>0.003388058859854937</v>
       </c>
       <c r="H14">
-        <v>0.0275275120511651</v>
+        <v>0.02714584022760391</v>
       </c>
       <c r="I14">
-        <v>0.001386471092700958</v>
+        <v>0.001327619422227144</v>
       </c>
       <c r="J14">
-        <v>0.00632206117734313</v>
+        <v>0.006429675035178661</v>
       </c>
       <c r="K14">
-        <v>0.002075059805065393</v>
+        <v>0.002142644021660089</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1107,28 +1107,28 @@
         <v>617</v>
       </c>
       <c r="D15">
-        <v>0.001198198180645704</v>
+        <v>0.001237661112099886</v>
       </c>
       <c r="E15">
-        <v>0.2847359217703342</v>
+        <v>0.2934476262889802</v>
       </c>
       <c r="F15">
         <v>617</v>
       </c>
       <c r="G15">
-        <v>0.02414836501702666</v>
+        <v>0.02473073313012719</v>
       </c>
       <c r="H15">
-        <v>0.1748937289230525</v>
+        <v>0.1807961696758866</v>
       </c>
       <c r="I15">
-        <v>0.01591190975159407</v>
+        <v>0.01601315708830953</v>
       </c>
       <c r="J15">
-        <v>0.03171652369201183</v>
+        <v>0.03334408765658736</v>
       </c>
       <c r="K15">
-        <v>0.01497953571379185</v>
+        <v>0.01546579273417592</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1137,10 +1137,10 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>4805</v>
       </c>
       <c r="E16">
-        <v>1.059409182518721</v>
+        <v>1.0750294579193</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1154,28 +1154,28 @@
         <v>97</v>
       </c>
       <c r="D17">
-        <v>0.002766044810414314</v>
+        <v>0.003100324422121048</v>
       </c>
       <c r="E17">
-        <v>0.05008273618295789</v>
+        <v>0.05447119008749723</v>
       </c>
       <c r="F17">
         <v>97</v>
       </c>
       <c r="G17">
-        <v>0.003728274255990982</v>
+        <v>0.003970513585954905</v>
       </c>
       <c r="H17">
-        <v>0.03120582643896341</v>
+        <v>0.03474805178120732</v>
       </c>
       <c r="I17">
-        <v>0.001357139553874731</v>
+        <v>0.001422002911567688</v>
       </c>
       <c r="J17">
-        <v>0.007799938321113586</v>
+        <v>0.008151958230882883</v>
       </c>
       <c r="K17">
-        <v>0.00234952662140131</v>
+        <v>0.002532115206122398</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1187,28 +1187,28 @@
         <v>691</v>
       </c>
       <c r="D18">
-        <v>0.002069283742457628</v>
+        <v>0.002204247750341892</v>
       </c>
       <c r="E18">
-        <v>0.3067218810319901</v>
+        <v>0.316681609954685</v>
       </c>
       <c r="F18">
         <v>691</v>
       </c>
       <c r="G18">
-        <v>0.02578407153487206</v>
+        <v>0.02525182301178575</v>
       </c>
       <c r="H18">
-        <v>0.1884060804732144</v>
+        <v>0.1976799173280597</v>
       </c>
       <c r="I18">
-        <v>0.01634280104190111</v>
+        <v>0.01706172991544008</v>
       </c>
       <c r="J18">
-        <v>0.03542019426822662</v>
+        <v>0.03536766255274415</v>
       </c>
       <c r="K18">
-        <v>0.01606227504089475</v>
+        <v>0.01633666781708598</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1220,28 +1220,28 @@
         <v>97</v>
       </c>
       <c r="D19">
-        <v>0.00293141882866621</v>
+        <v>0.003161663189530373</v>
       </c>
       <c r="E19">
-        <v>0.05188515409827232</v>
+        <v>0.05682329786941409</v>
       </c>
       <c r="F19">
         <v>97</v>
       </c>
       <c r="G19">
-        <v>0.00397630175575614</v>
+        <v>0.004329751711338758</v>
       </c>
       <c r="H19">
-        <v>0.03239032998681068</v>
+        <v>0.0365743669681251</v>
       </c>
       <c r="I19">
-        <v>0.001482035033404827</v>
+        <v>0.001428878866136074</v>
       </c>
       <c r="J19">
-        <v>0.008001338224858046</v>
+        <v>0.008125264663249254</v>
       </c>
       <c r="K19">
-        <v>0.002349940128624439</v>
+        <v>0.002553056925535202</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1253,28 +1253,28 @@
         <v>691</v>
       </c>
       <c r="D20">
-        <v>0.001264994964003563</v>
+        <v>0.001299806404858828</v>
       </c>
       <c r="E20">
-        <v>0.300749619025737</v>
+        <v>0.3178509171120822</v>
       </c>
       <c r="F20">
         <v>691</v>
       </c>
       <c r="G20">
-        <v>0.0252198320813477</v>
+        <v>0.02665189374238253</v>
       </c>
       <c r="H20">
-        <v>0.1854279190301895</v>
+        <v>0.1965084415860474</v>
       </c>
       <c r="I20">
-        <v>0.01708532124757767</v>
+        <v>0.01769693940877914</v>
       </c>
       <c r="J20">
-        <v>0.03404026012867689</v>
+        <v>0.03630434768274426</v>
       </c>
       <c r="K20">
-        <v>0.01527096331119537</v>
+        <v>0.01606337446719408</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1283,10 +1283,10 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>4805</v>
       </c>
       <c r="E21">
-        <v>1.00795480562374</v>
+        <v>1.042856383603066</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1300,28 +1300,28 @@
         <v>80</v>
       </c>
       <c r="D22">
-        <v>0.002676998730748892</v>
+        <v>0.002818004693835974</v>
       </c>
       <c r="E22">
-        <v>0.04325457895174623</v>
+        <v>0.04500549519434571</v>
       </c>
       <c r="F22">
         <v>80</v>
       </c>
       <c r="G22">
-        <v>0.003306585364043713</v>
+        <v>0.00331448158249259</v>
       </c>
       <c r="H22">
-        <v>0.02701234305277467</v>
+        <v>0.027995181735605</v>
       </c>
       <c r="I22">
-        <v>0.00129800708964467</v>
+        <v>0.001283865422010422</v>
       </c>
       <c r="J22">
-        <v>0.006706702057272196</v>
+        <v>0.007226055953651667</v>
       </c>
       <c r="K22">
-        <v>0.001983508002012968</v>
+        <v>0.002052519004791975</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1333,28 +1333,28 @@
         <v>645</v>
       </c>
       <c r="D23">
-        <v>0.001876875292509794</v>
+        <v>0.002064861822873354</v>
       </c>
       <c r="E23">
-        <v>0.2856964897364378</v>
+        <v>0.2926517301239073</v>
       </c>
       <c r="F23">
         <v>645</v>
       </c>
       <c r="G23">
-        <v>0.02377653401345015</v>
+        <v>0.02392783807590604</v>
       </c>
       <c r="H23">
-        <v>0.1768475039862096</v>
+        <v>0.1824900843203068</v>
       </c>
       <c r="I23">
-        <v>0.01542425900697708</v>
+        <v>0.01616172399371862</v>
       </c>
       <c r="J23">
-        <v>0.0322994259186089</v>
+        <v>0.03163070045411587</v>
       </c>
       <c r="K23">
-        <v>0.01486537978053093</v>
+        <v>0.01501797046512365</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1366,28 +1366,28 @@
         <v>80</v>
       </c>
       <c r="D24">
-        <v>0.002617469057440758</v>
+        <v>0.002560560591518879</v>
       </c>
       <c r="E24">
-        <v>0.04459123313426971</v>
+        <v>0.04559829970821738</v>
       </c>
       <c r="F24">
         <v>80</v>
       </c>
       <c r="G24">
-        <v>0.003365387208759785</v>
+        <v>0.003526780288666487</v>
       </c>
       <c r="H24">
-        <v>0.0278595769777894</v>
+        <v>0.02853199047967792</v>
       </c>
       <c r="I24">
-        <v>0.001256630290299654</v>
+        <v>0.001291815191507339</v>
       </c>
       <c r="J24">
-        <v>0.006917370017617941</v>
+        <v>0.007153824437409639</v>
       </c>
       <c r="K24">
-        <v>0.002033184748142958</v>
+        <v>0.002053318545222282</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1399,28 +1399,28 @@
         <v>645</v>
       </c>
       <c r="D25">
-        <v>0.00120099913328886</v>
+        <v>0.001223662402480841</v>
       </c>
       <c r="E25">
-        <v>0.2911525252275169</v>
+        <v>0.3002450447529554</v>
       </c>
       <c r="F25">
         <v>645</v>
       </c>
       <c r="G25">
-        <v>0.02450546575710177</v>
+        <v>0.02534763514995575</v>
       </c>
       <c r="H25">
-        <v>0.178148933686316</v>
+        <v>0.1827242709696293</v>
       </c>
       <c r="I25">
-        <v>0.01639682101085782</v>
+        <v>0.01744035072624683</v>
       </c>
       <c r="J25">
-        <v>0.03340143710374832</v>
+        <v>0.03507415438070893</v>
       </c>
       <c r="K25">
-        <v>0.0150182475335896</v>
+        <v>0.01557184895500541</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1429,10 +1429,10 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>4805</v>
       </c>
       <c r="E26">
-        <v>0.8913419921882451</v>
+        <v>1.037118395324796</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1446,28 +1446,28 @@
         <v>84.8</v>
       </c>
       <c r="D27">
-        <v>0.002881017979234457</v>
+        <v>0.003170470520853996</v>
       </c>
       <c r="E27">
-        <v>0.04731297260150313</v>
+        <v>0.05335342586040497</v>
       </c>
       <c r="F27">
         <v>84.8</v>
       </c>
       <c r="G27">
-        <v>0.003563164547085762</v>
+        <v>0.003871057648211718</v>
       </c>
       <c r="H27">
-        <v>0.02966500939801335</v>
+        <v>0.03343966268002987</v>
       </c>
       <c r="I27">
-        <v>0.00131884329020977</v>
+        <v>0.001487807743251324</v>
       </c>
       <c r="J27">
-        <v>0.007273943442851305</v>
+        <v>0.008378754742443562</v>
       </c>
       <c r="K27">
-        <v>0.002179708518087864</v>
+        <v>0.002440508455038071</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1479,28 +1479,28 @@
         <v>695.6</v>
       </c>
       <c r="D28">
-        <v>0.002048211079090834</v>
+        <v>0.002239363081753254</v>
       </c>
       <c r="E28">
-        <v>0.3053763858042657</v>
+        <v>0.3182877928949893</v>
       </c>
       <c r="F28">
         <v>695.6</v>
       </c>
       <c r="G28">
-        <v>0.02566413339227438</v>
+        <v>0.02590213250368834</v>
       </c>
       <c r="H28">
-        <v>0.1888218046166003</v>
+        <v>0.1983522991649806</v>
       </c>
       <c r="I28">
-        <v>0.01568729383870959</v>
+        <v>0.01677891565486789</v>
       </c>
       <c r="J28">
-        <v>0.03470656583085656</v>
+        <v>0.03523902604356408</v>
       </c>
       <c r="K28">
-        <v>0.01594782778993249</v>
+        <v>0.01652187332510948</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1512,28 +1512,28 @@
         <v>84.8</v>
       </c>
       <c r="D29">
-        <v>0.002732870448380709</v>
+        <v>0.002964556869119406</v>
       </c>
       <c r="E29">
-        <v>0.04710490815341473</v>
+        <v>0.05446625016629696</v>
       </c>
       <c r="F29">
         <v>84.8</v>
       </c>
       <c r="G29">
-        <v>0.003601891826838255</v>
+        <v>0.004190443921834231</v>
       </c>
       <c r="H29">
-        <v>0.02947240518406034</v>
+        <v>0.03420430552214384</v>
       </c>
       <c r="I29">
-        <v>0.001363600417971611</v>
+        <v>0.001460702531039715</v>
       </c>
       <c r="J29">
-        <v>0.007241168897598982</v>
+        <v>0.008357279933989048</v>
       </c>
       <c r="K29">
-        <v>0.002115057408809662</v>
+        <v>0.002514432184398174</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1545,28 +1545,28 @@
         <v>695.6</v>
       </c>
       <c r="D30">
-        <v>0.001279656123369932</v>
+        <v>0.001341995317488909</v>
       </c>
       <c r="E30">
-        <v>0.3061636821366847</v>
+        <v>0.3257415600121021</v>
       </c>
       <c r="F30">
         <v>695.6</v>
       </c>
       <c r="G30">
-        <v>0.02588624712079763</v>
+        <v>0.02771347779780626</v>
       </c>
       <c r="H30">
-        <v>0.1882273947820067</v>
+        <v>0.2007194611243904</v>
       </c>
       <c r="I30">
-        <v>0.01667132312431931</v>
+        <v>0.01760063720867038</v>
       </c>
       <c r="J30">
-        <v>0.03472918085753918</v>
+        <v>0.03716497588902712</v>
       </c>
       <c r="K30">
-        <v>0.01593796070665121</v>
+        <v>0.01685742549598217</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1575,10 +1575,10 @@
         <v>25</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>4805</v>
       </c>
       <c r="E31">
-        <v>0.9926352506503463</v>
+        <v>1.09639613237232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>